<commit_message>
add monster data table
</commit_message>
<xml_diff>
--- a/Assets/ExcelDataTables/MonsterData.xlsx
+++ b/Assets/ExcelDataTables/MonsterData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UnityProject\UnityKoreaAward\Assets\ExcelDataTables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9F341A5-111D-4831-A547-F38C288057E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45C4C3D1-2DD3-4E10-8CC2-E25570AA5E43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1935" yWindow="765" windowWidth="26505" windowHeight="14565" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="16200" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MonsterBaseData" sheetId="1" r:id="rId1"/>
@@ -507,7 +507,7 @@
     <author>신성환</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{FB2996C2-D567-446C-85E6-C3D24007A297}">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{93990E13-2B9D-440D-8F65-0A98CC170704}">
       <text>
         <r>
           <rPr>
@@ -759,6 +759,47 @@
             <charset val="129"/>
           </rPr>
           <t>추가</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{5DB58EB3-9EEC-4E09-8394-3D6DA479FDCC}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>신성환</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t xml:space="preserve">곱연산
+체력
+공격력
+경험치
+</t>
         </r>
       </text>
     </comment>
@@ -932,7 +973,7 @@
     <author>신성환</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{8DFAD599-2F45-48A1-B515-8F7B4CAE4B70}">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{DB83A69D-A847-4E47-9636-AAAE7C6F87E1}">
       <text>
         <r>
           <rPr>
@@ -1184,6 +1225,47 @@
             <charset val="129"/>
           </rPr>
           <t>추가</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{1820DCF1-D7E7-4F00-B9BC-41754E940027}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>신성환</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t xml:space="preserve">곱연산
+체력
+공격력
+경험치
+</t>
         </r>
       </text>
     </comment>
@@ -1777,7 +1859,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="18">
   <si>
     <t>PlayerSkillType DropBox List</t>
   </si>
@@ -1794,9 +1876,6 @@
     <t>Skill Type</t>
   </si>
   <si>
-    <t>NumberOfBullets::int</t>
-  </si>
-  <si>
     <t>HP::int</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
@@ -1810,10 +1889,6 @@
   </si>
   <si>
     <t>MonsterSkiilsType::enum</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>RangeOfFire::float</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
@@ -1834,6 +1909,22 @@
   </si>
   <si>
     <t>MonsterSkiilsType DropBox List</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>MeleeMonstser</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>RangedMonster</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>MonsterType::string</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>HP::float</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
@@ -1950,13 +2041,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2360,11 +2451,11 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:N40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="75" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="L21" sqref="L21"/>
+      <selection pane="bottomRight" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2390,7 +2481,7 @@
         <v>3</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
@@ -2399,29 +2490,29 @@
         <v>2</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="5" t="s">
-        <v>8</v>
-      </c>
       <c r="J1" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="K1" s="2"/>
       <c r="M1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="N1" s="8" t="s">
-        <v>15</v>
+      <c r="N1" s="6" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
@@ -2447,7 +2538,7 @@
       <c r="J2" s="1">
         <v>10</v>
       </c>
-      <c r="M2" s="6"/>
+      <c r="M2" s="7"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
@@ -2472,7 +2563,7 @@
       <c r="J3" s="1">
         <v>11</v>
       </c>
-      <c r="M3" s="6"/>
+      <c r="M3" s="7"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
@@ -2497,7 +2588,7 @@
       <c r="J4" s="1">
         <v>12</v>
       </c>
-      <c r="M4" s="6"/>
+      <c r="M4" s="7"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
@@ -2522,7 +2613,7 @@
       <c r="J5" s="1">
         <v>13</v>
       </c>
-      <c r="M5" s="6"/>
+      <c r="M5" s="7"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
@@ -2547,7 +2638,7 @@
       <c r="J6" s="1">
         <v>14</v>
       </c>
-      <c r="M6" s="6"/>
+      <c r="M6" s="7"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
@@ -2572,7 +2663,7 @@
       <c r="J7" s="1">
         <v>15</v>
       </c>
-      <c r="M7" s="6"/>
+      <c r="M7" s="7"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
@@ -2597,7 +2688,7 @@
       <c r="J8" s="1">
         <v>16</v>
       </c>
-      <c r="M8" s="6"/>
+      <c r="M8" s="7"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
@@ -2622,7 +2713,7 @@
       <c r="J9" s="1">
         <v>17</v>
       </c>
-      <c r="M9" s="7"/>
+      <c r="M9" s="8"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
@@ -2647,7 +2738,7 @@
       <c r="J10" s="1">
         <v>18</v>
       </c>
-      <c r="M10" s="7"/>
+      <c r="M10" s="8"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
@@ -2672,7 +2763,7 @@
       <c r="J11" s="1">
         <v>19</v>
       </c>
-      <c r="M11" s="7"/>
+      <c r="M11" s="8"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
@@ -2697,7 +2788,7 @@
       <c r="J12" s="1">
         <v>20</v>
       </c>
-      <c r="M12" s="7"/>
+      <c r="M12" s="8"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
@@ -2722,7 +2813,7 @@
       <c r="J13" s="1">
         <v>21</v>
       </c>
-      <c r="M13" s="7"/>
+      <c r="M13" s="8"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
@@ -2747,7 +2838,7 @@
       <c r="J14" s="1">
         <v>22</v>
       </c>
-      <c r="M14" s="7"/>
+      <c r="M14" s="8"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
@@ -3368,10 +3459,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{538B65EF-D419-4214-A215-575E19AD76B9}">
-  <dimension ref="A1:L14"/>
+  <dimension ref="A1:L57"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3379,13 +3470,13 @@
     <col min="1" max="1" width="6.125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.75" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.375" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.5" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.5" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.25" style="1" customWidth="1"/>
-    <col min="10" max="10" width="17.5" style="1" customWidth="1"/>
+    <col min="9" max="9" width="15.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.75" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.625" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="32.875" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="16384" width="9" style="1"/>
@@ -3396,27 +3487,32 @@
         <v>3</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
+      <c r="D1" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="E1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I1" s="2"/>
+      <c r="J1" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="K1" s="1" t="s">
         <v>4</v>
       </c>
@@ -3426,94 +3522,1393 @@
     </row>
     <row r="2" spans="1:12" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
+        <f>MonsterBaseData!A2</f>
         <v>1</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="K2" s="6"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="1">
+        <f>MonsterBaseData!E2</f>
+        <v>1</v>
+      </c>
+      <c r="F2" s="1">
+        <f>MonsterBaseData!F2</f>
+        <v>10</v>
+      </c>
+      <c r="G2" s="1">
+        <f>MonsterBaseData!G2*1.5</f>
+        <v>15</v>
+      </c>
+      <c r="H2" s="1">
+        <f>MonsterBaseData!H2</f>
+        <v>0.5</v>
+      </c>
+      <c r="I2" s="1">
+        <f>MonsterBaseData!I2</f>
+        <v>0.3</v>
+      </c>
+      <c r="J2" s="1">
+        <f>MonsterBaseData!J2*1.5</f>
+        <v>15</v>
+      </c>
+      <c r="K2" s="7"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
+        <f>MonsterBaseData!A3</f>
         <v>2</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="K3" s="6"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="1">
+        <f>MonsterBaseData!E3</f>
+        <v>2</v>
+      </c>
+      <c r="F3" s="1">
+        <f>MonsterBaseData!F3</f>
+        <v>15</v>
+      </c>
+      <c r="G3" s="1">
+        <f>MonsterBaseData!G3*1.5</f>
+        <v>22.5</v>
+      </c>
+      <c r="H3" s="1">
+        <f>MonsterBaseData!H3</f>
+        <v>0.52500000000000002</v>
+      </c>
+      <c r="I3" s="1">
+        <f>MonsterBaseData!I3</f>
+        <v>0.35</v>
+      </c>
+      <c r="J3" s="1">
+        <f>MonsterBaseData!J3*1.5</f>
+        <v>16.5</v>
+      </c>
+      <c r="K3" s="7"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
+        <f>MonsterBaseData!A4</f>
         <v>3</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="K4" s="6"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="1">
+        <f>MonsterBaseData!E4</f>
+        <v>3</v>
+      </c>
+      <c r="F4" s="1">
+        <f>MonsterBaseData!F4</f>
+        <v>20</v>
+      </c>
+      <c r="G4" s="1">
+        <f>MonsterBaseData!G4*1.5</f>
+        <v>30</v>
+      </c>
+      <c r="H4" s="1">
+        <f>MonsterBaseData!H4</f>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="I4" s="1">
+        <f>MonsterBaseData!I4</f>
+        <v>0.4</v>
+      </c>
+      <c r="J4" s="1">
+        <f>MonsterBaseData!J4*1.5</f>
+        <v>18</v>
+      </c>
+      <c r="K4" s="7"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
+        <f>MonsterBaseData!A5</f>
         <v>4</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="K5" s="6"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="1">
+        <f>MonsterBaseData!E5</f>
+        <v>4</v>
+      </c>
+      <c r="F5" s="1">
+        <f>MonsterBaseData!F5</f>
+        <v>25</v>
+      </c>
+      <c r="G5" s="1">
+        <f>MonsterBaseData!G5*1.5</f>
+        <v>37.5</v>
+      </c>
+      <c r="H5" s="1">
+        <f>MonsterBaseData!H5</f>
+        <v>0.57499999999999996</v>
+      </c>
+      <c r="I5" s="1">
+        <f>MonsterBaseData!I5</f>
+        <v>0.45</v>
+      </c>
+      <c r="J5" s="1">
+        <f>MonsterBaseData!J5*1.5</f>
+        <v>19.5</v>
+      </c>
+      <c r="K5" s="7"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
+        <f>MonsterBaseData!A6</f>
         <v>5</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="K6" s="6"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="1">
+        <f>MonsterBaseData!E6</f>
+        <v>5</v>
+      </c>
+      <c r="F6" s="1">
+        <f>MonsterBaseData!F6</f>
+        <v>30</v>
+      </c>
+      <c r="G6" s="1">
+        <f>MonsterBaseData!G6*1.5</f>
+        <v>45</v>
+      </c>
+      <c r="H6" s="1">
+        <f>MonsterBaseData!H6</f>
+        <v>0.6</v>
+      </c>
+      <c r="I6" s="1">
+        <f>MonsterBaseData!I6</f>
+        <v>0.5</v>
+      </c>
+      <c r="J6" s="1">
+        <f>MonsterBaseData!J6*1.5</f>
+        <v>21</v>
+      </c>
+      <c r="K6" s="7"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
+        <f>MonsterBaseData!A7</f>
         <v>6</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="K7" s="6"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="1">
+        <f>MonsterBaseData!E7</f>
+        <v>6</v>
+      </c>
+      <c r="F7" s="1">
+        <f>MonsterBaseData!F7</f>
+        <v>35</v>
+      </c>
+      <c r="G7" s="1">
+        <f>MonsterBaseData!G7*1.5</f>
+        <v>52.5</v>
+      </c>
+      <c r="H7" s="1">
+        <f>MonsterBaseData!H7</f>
+        <v>0.625</v>
+      </c>
+      <c r="I7" s="1">
+        <f>MonsterBaseData!I7</f>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="J7" s="1">
+        <f>MonsterBaseData!J7*1.5</f>
+        <v>22.5</v>
+      </c>
+      <c r="K7" s="7"/>
     </row>
     <row r="8" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
+        <f>MonsterBaseData!A8</f>
         <v>7</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="K8" s="6"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="1">
+        <f>MonsterBaseData!E8</f>
+        <v>7</v>
+      </c>
+      <c r="F8" s="1">
+        <f>MonsterBaseData!F8</f>
+        <v>40</v>
+      </c>
+      <c r="G8" s="1">
+        <f>MonsterBaseData!G8*1.5</f>
+        <v>60</v>
+      </c>
+      <c r="H8" s="1">
+        <f>MonsterBaseData!H8</f>
+        <v>0.65</v>
+      </c>
+      <c r="I8" s="1">
+        <f>MonsterBaseData!I8</f>
+        <v>0.6</v>
+      </c>
+      <c r="J8" s="1">
+        <f>MonsterBaseData!J8*1.5</f>
+        <v>24</v>
+      </c>
+      <c r="K8" s="7"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
+        <f>MonsterBaseData!A9</f>
         <v>8</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="K9" s="7"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="1">
+        <f>MonsterBaseData!E9</f>
+        <v>8</v>
+      </c>
+      <c r="F9" s="1">
+        <f>MonsterBaseData!F9</f>
+        <v>45</v>
+      </c>
+      <c r="G9" s="1">
+        <f>MonsterBaseData!G9*1.5</f>
+        <v>67.5</v>
+      </c>
+      <c r="H9" s="1">
+        <f>MonsterBaseData!H9</f>
+        <v>0.67500000000000004</v>
+      </c>
+      <c r="I9" s="1">
+        <f>MonsterBaseData!I9</f>
+        <v>0.65</v>
+      </c>
+      <c r="J9" s="1">
+        <f>MonsterBaseData!J9*1.5</f>
+        <v>25.5</v>
+      </c>
+      <c r="K9" s="8"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
+        <f>MonsterBaseData!A10</f>
         <v>9</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="K10" s="7"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="1">
+        <f>MonsterBaseData!E10</f>
+        <v>9</v>
+      </c>
+      <c r="F10" s="1">
+        <f>MonsterBaseData!F10</f>
+        <v>50</v>
+      </c>
+      <c r="G10" s="1">
+        <f>MonsterBaseData!G10*1.5</f>
+        <v>75</v>
+      </c>
+      <c r="H10" s="1">
+        <f>MonsterBaseData!H10</f>
+        <v>0.7</v>
+      </c>
+      <c r="I10" s="1">
+        <f>MonsterBaseData!I10</f>
+        <v>0.7</v>
+      </c>
+      <c r="J10" s="1">
+        <f>MonsterBaseData!J10*1.5</f>
+        <v>27</v>
+      </c>
+      <c r="K10" s="8"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
+        <f>MonsterBaseData!A11</f>
         <v>10</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="K11" s="7"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="1">
+        <f>MonsterBaseData!E11</f>
+        <v>10</v>
+      </c>
+      <c r="F11" s="1">
+        <f>MonsterBaseData!F11</f>
+        <v>55</v>
+      </c>
+      <c r="G11" s="1">
+        <f>MonsterBaseData!G11*1.5</f>
+        <v>82.5</v>
+      </c>
+      <c r="H11" s="1">
+        <f>MonsterBaseData!H11</f>
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="I11" s="1">
+        <f>MonsterBaseData!I11</f>
+        <v>0.75</v>
+      </c>
+      <c r="J11" s="1">
+        <f>MonsterBaseData!J11*1.5</f>
+        <v>28.5</v>
+      </c>
+      <c r="K11" s="8"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
+        <f>MonsterBaseData!A12</f>
         <v>11</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="K12" s="7"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="1">
+        <f>MonsterBaseData!E12</f>
+        <v>11</v>
+      </c>
+      <c r="F12" s="1">
+        <f>MonsterBaseData!F12</f>
+        <v>60</v>
+      </c>
+      <c r="G12" s="1">
+        <f>MonsterBaseData!G12*1.5</f>
+        <v>90</v>
+      </c>
+      <c r="H12" s="1">
+        <f>MonsterBaseData!H12</f>
+        <v>0.75</v>
+      </c>
+      <c r="I12" s="1">
+        <f>MonsterBaseData!I12</f>
+        <v>0.8</v>
+      </c>
+      <c r="J12" s="1">
+        <f>MonsterBaseData!J12*1.5</f>
+        <v>30</v>
+      </c>
+      <c r="K12" s="8"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
+        <f>MonsterBaseData!A13</f>
         <v>12</v>
       </c>
-      <c r="C13" s="4"/>
-      <c r="K13" s="7"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="1">
+        <f>MonsterBaseData!E13</f>
+        <v>12</v>
+      </c>
+      <c r="F13" s="1">
+        <f>MonsterBaseData!F13</f>
+        <v>65</v>
+      </c>
+      <c r="G13" s="1">
+        <f>MonsterBaseData!G13*1.5</f>
+        <v>97.5</v>
+      </c>
+      <c r="H13" s="1">
+        <f>MonsterBaseData!H13</f>
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="I13" s="1">
+        <f>MonsterBaseData!I13</f>
+        <v>0.85</v>
+      </c>
+      <c r="J13" s="1">
+        <f>MonsterBaseData!J13*1.5</f>
+        <v>31.5</v>
+      </c>
+      <c r="K13" s="8"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
+        <f>MonsterBaseData!A14</f>
         <v>13</v>
       </c>
-      <c r="C14" s="4"/>
-      <c r="K14" s="7"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="1">
+        <f>MonsterBaseData!E14</f>
+        <v>13</v>
+      </c>
+      <c r="F14" s="1">
+        <f>MonsterBaseData!F14</f>
+        <v>70</v>
+      </c>
+      <c r="G14" s="1">
+        <f>MonsterBaseData!G14*1.5</f>
+        <v>105</v>
+      </c>
+      <c r="H14" s="1">
+        <f>MonsterBaseData!H14</f>
+        <v>0.8</v>
+      </c>
+      <c r="I14" s="1">
+        <f>MonsterBaseData!I14</f>
+        <v>0.9</v>
+      </c>
+      <c r="J14" s="1">
+        <f>MonsterBaseData!J14*1.5</f>
+        <v>33</v>
+      </c>
+      <c r="K14" s="8"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <f>MonsterBaseData!A15</f>
+        <v>14</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="D15" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" s="1">
+        <f>MonsterBaseData!E15</f>
+        <v>14</v>
+      </c>
+      <c r="F15" s="1">
+        <f>MonsterBaseData!F15</f>
+        <v>75</v>
+      </c>
+      <c r="G15" s="1">
+        <f>MonsterBaseData!G15*1.5</f>
+        <v>112.5</v>
+      </c>
+      <c r="H15" s="1">
+        <f>MonsterBaseData!H15</f>
+        <v>0.82499999999999996</v>
+      </c>
+      <c r="I15" s="1">
+        <f>MonsterBaseData!I15</f>
+        <v>0.95</v>
+      </c>
+      <c r="J15" s="1">
+        <f>MonsterBaseData!J15*1.5</f>
+        <v>34.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <f>MonsterBaseData!A16</f>
+        <v>15</v>
+      </c>
+      <c r="C16" s="1"/>
+      <c r="D16" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" s="1">
+        <f>MonsterBaseData!E16</f>
+        <v>15</v>
+      </c>
+      <c r="F16" s="1">
+        <f>MonsterBaseData!F16</f>
+        <v>80</v>
+      </c>
+      <c r="G16" s="1">
+        <f>MonsterBaseData!G16*1.5</f>
+        <v>120</v>
+      </c>
+      <c r="H16" s="1">
+        <f>MonsterBaseData!H16</f>
+        <v>0.85</v>
+      </c>
+      <c r="I16" s="1">
+        <f>MonsterBaseData!I16</f>
+        <v>1</v>
+      </c>
+      <c r="J16" s="1">
+        <f>MonsterBaseData!J16*1.5</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <f>MonsterBaseData!A17</f>
+        <v>16</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="D17" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" s="1">
+        <f>MonsterBaseData!E17</f>
+        <v>16</v>
+      </c>
+      <c r="F17" s="1">
+        <f>MonsterBaseData!F17</f>
+        <v>85</v>
+      </c>
+      <c r="G17" s="1">
+        <f>MonsterBaseData!G17*1.5</f>
+        <v>127.5</v>
+      </c>
+      <c r="H17" s="1">
+        <f>MonsterBaseData!H17</f>
+        <v>0.875</v>
+      </c>
+      <c r="I17" s="1">
+        <f>MonsterBaseData!I17</f>
+        <v>1.05</v>
+      </c>
+      <c r="J17" s="1">
+        <f>MonsterBaseData!J17*1.5</f>
+        <v>37.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <f>MonsterBaseData!A18</f>
+        <v>17</v>
+      </c>
+      <c r="C18" s="1"/>
+      <c r="D18" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" s="1">
+        <f>MonsterBaseData!E18</f>
+        <v>17</v>
+      </c>
+      <c r="F18" s="1">
+        <f>MonsterBaseData!F18</f>
+        <v>90</v>
+      </c>
+      <c r="G18" s="1">
+        <f>MonsterBaseData!G18*1.5</f>
+        <v>135</v>
+      </c>
+      <c r="H18" s="1">
+        <f>MonsterBaseData!H18</f>
+        <v>0.9</v>
+      </c>
+      <c r="I18" s="1">
+        <f>MonsterBaseData!I18</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="J18" s="1">
+        <f>MonsterBaseData!J18*1.5</f>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <f>MonsterBaseData!A19</f>
+        <v>18</v>
+      </c>
+      <c r="C19" s="1"/>
+      <c r="D19" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E19" s="1">
+        <f>MonsterBaseData!E19</f>
+        <v>18</v>
+      </c>
+      <c r="F19" s="1">
+        <f>MonsterBaseData!F19</f>
+        <v>95</v>
+      </c>
+      <c r="G19" s="1">
+        <f>MonsterBaseData!G19*1.5</f>
+        <v>142.5</v>
+      </c>
+      <c r="H19" s="1">
+        <f>MonsterBaseData!H19</f>
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="I19" s="1">
+        <f>MonsterBaseData!I19</f>
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="J19" s="1">
+        <f>MonsterBaseData!J19*1.5</f>
+        <v>40.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <f>MonsterBaseData!A20</f>
+        <v>19</v>
+      </c>
+      <c r="C20" s="1"/>
+      <c r="D20" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20" s="1">
+        <f>MonsterBaseData!E20</f>
+        <v>19</v>
+      </c>
+      <c r="F20" s="1">
+        <f>MonsterBaseData!F20</f>
+        <v>100</v>
+      </c>
+      <c r="G20" s="1">
+        <f>MonsterBaseData!G20*1.5</f>
+        <v>150</v>
+      </c>
+      <c r="H20" s="1">
+        <f>MonsterBaseData!H20</f>
+        <v>0.95</v>
+      </c>
+      <c r="I20" s="1">
+        <f>MonsterBaseData!I20</f>
+        <v>1.2</v>
+      </c>
+      <c r="J20" s="1">
+        <f>MonsterBaseData!J20*1.5</f>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <f>MonsterBaseData!A21</f>
+        <v>20</v>
+      </c>
+      <c r="C21" s="1"/>
+      <c r="D21" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21" s="1">
+        <f>MonsterBaseData!E21</f>
+        <v>20</v>
+      </c>
+      <c r="F21" s="1">
+        <f>MonsterBaseData!F21</f>
+        <v>105</v>
+      </c>
+      <c r="G21" s="1">
+        <f>MonsterBaseData!G21*1.5</f>
+        <v>157.5</v>
+      </c>
+      <c r="H21" s="1">
+        <f>MonsterBaseData!H21</f>
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="I21" s="1">
+        <f>MonsterBaseData!I21</f>
+        <v>1.25</v>
+      </c>
+      <c r="J21" s="1">
+        <f>MonsterBaseData!J21*1.5</f>
+        <v>43.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <f>MonsterBaseData!A22</f>
+        <v>21</v>
+      </c>
+      <c r="C22" s="1"/>
+      <c r="D22" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22" s="1">
+        <f>MonsterBaseData!E22</f>
+        <v>21</v>
+      </c>
+      <c r="F22" s="1">
+        <f>MonsterBaseData!F22</f>
+        <v>110</v>
+      </c>
+      <c r="G22" s="1">
+        <f>MonsterBaseData!G22*1.5</f>
+        <v>165</v>
+      </c>
+      <c r="H22" s="1">
+        <f>MonsterBaseData!H22</f>
+        <v>1</v>
+      </c>
+      <c r="I22" s="1">
+        <f>MonsterBaseData!I22</f>
+        <v>1.3</v>
+      </c>
+      <c r="J22" s="1">
+        <f>MonsterBaseData!J22*1.5</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <f>MonsterBaseData!A23</f>
+        <v>22</v>
+      </c>
+      <c r="C23" s="1"/>
+      <c r="D23" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E23" s="1">
+        <f>MonsterBaseData!E23</f>
+        <v>22</v>
+      </c>
+      <c r="F23" s="1">
+        <f>MonsterBaseData!F23</f>
+        <v>115</v>
+      </c>
+      <c r="G23" s="1">
+        <f>MonsterBaseData!G23*1.5</f>
+        <v>172.5</v>
+      </c>
+      <c r="H23" s="1">
+        <f>MonsterBaseData!H23</f>
+        <v>1.0249999999999999</v>
+      </c>
+      <c r="I23" s="1">
+        <f>MonsterBaseData!I23</f>
+        <v>1.35</v>
+      </c>
+      <c r="J23" s="1">
+        <f>MonsterBaseData!J23*1.5</f>
+        <v>46.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <f>MonsterBaseData!A24</f>
+        <v>23</v>
+      </c>
+      <c r="C24" s="1"/>
+      <c r="D24" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E24" s="1">
+        <f>MonsterBaseData!E24</f>
+        <v>23</v>
+      </c>
+      <c r="F24" s="1">
+        <f>MonsterBaseData!F24</f>
+        <v>120</v>
+      </c>
+      <c r="G24" s="1">
+        <f>MonsterBaseData!G24*1.5</f>
+        <v>180</v>
+      </c>
+      <c r="H24" s="1">
+        <f>MonsterBaseData!H24</f>
+        <v>1.05</v>
+      </c>
+      <c r="I24" s="1">
+        <f>MonsterBaseData!I24</f>
+        <v>1.4</v>
+      </c>
+      <c r="J24" s="1">
+        <f>MonsterBaseData!J24*1.5</f>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <f>MonsterBaseData!A25</f>
+        <v>24</v>
+      </c>
+      <c r="C25" s="1"/>
+      <c r="D25" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E25" s="1">
+        <f>MonsterBaseData!E25</f>
+        <v>24</v>
+      </c>
+      <c r="F25" s="1">
+        <f>MonsterBaseData!F25</f>
+        <v>125</v>
+      </c>
+      <c r="G25" s="1">
+        <f>MonsterBaseData!G25*1.5</f>
+        <v>187.5</v>
+      </c>
+      <c r="H25" s="1">
+        <f>MonsterBaseData!H25</f>
+        <v>1.075</v>
+      </c>
+      <c r="I25" s="1">
+        <f>MonsterBaseData!I25</f>
+        <v>1.45</v>
+      </c>
+      <c r="J25" s="1">
+        <f>MonsterBaseData!J25*1.5</f>
+        <v>49.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
+        <f>MonsterBaseData!A26</f>
+        <v>25</v>
+      </c>
+      <c r="C26" s="1"/>
+      <c r="D26" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E26" s="1">
+        <f>MonsterBaseData!E26</f>
+        <v>25</v>
+      </c>
+      <c r="F26" s="1">
+        <f>MonsterBaseData!F26</f>
+        <v>130</v>
+      </c>
+      <c r="G26" s="1">
+        <f>MonsterBaseData!G26*1.5</f>
+        <v>195</v>
+      </c>
+      <c r="H26" s="1">
+        <f>MonsterBaseData!H26</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="I26" s="1">
+        <f>MonsterBaseData!I26</f>
+        <v>1.5</v>
+      </c>
+      <c r="J26" s="1">
+        <f>MonsterBaseData!J26*1.5</f>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <f>MonsterBaseData!A27</f>
+        <v>26</v>
+      </c>
+      <c r="C27" s="1"/>
+      <c r="D27" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E27" s="1">
+        <f>MonsterBaseData!E27</f>
+        <v>26</v>
+      </c>
+      <c r="F27" s="1">
+        <f>MonsterBaseData!F27</f>
+        <v>135</v>
+      </c>
+      <c r="G27" s="1">
+        <f>MonsterBaseData!G27*1.5</f>
+        <v>202.5</v>
+      </c>
+      <c r="H27" s="1">
+        <f>MonsterBaseData!H27</f>
+        <v>1.125</v>
+      </c>
+      <c r="I27" s="1">
+        <f>MonsterBaseData!I27</f>
+        <v>1.55</v>
+      </c>
+      <c r="J27" s="1">
+        <f>MonsterBaseData!J27*1.5</f>
+        <v>52.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
+        <f>MonsterBaseData!A28</f>
+        <v>27</v>
+      </c>
+      <c r="C28" s="1"/>
+      <c r="D28" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E28" s="1">
+        <f>MonsterBaseData!E28</f>
+        <v>27</v>
+      </c>
+      <c r="F28" s="1">
+        <f>MonsterBaseData!F28</f>
+        <v>140</v>
+      </c>
+      <c r="G28" s="1">
+        <f>MonsterBaseData!G28*1.5</f>
+        <v>210</v>
+      </c>
+      <c r="H28" s="1">
+        <f>MonsterBaseData!H28</f>
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="I28" s="1">
+        <f>MonsterBaseData!I28</f>
+        <v>1.6</v>
+      </c>
+      <c r="J28" s="1">
+        <f>MonsterBaseData!J28*1.5</f>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
+        <f>MonsterBaseData!A29</f>
+        <v>28</v>
+      </c>
+      <c r="C29" s="1"/>
+      <c r="D29" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E29" s="1">
+        <f>MonsterBaseData!E29</f>
+        <v>28</v>
+      </c>
+      <c r="F29" s="1">
+        <f>MonsterBaseData!F29</f>
+        <v>145</v>
+      </c>
+      <c r="G29" s="1">
+        <f>MonsterBaseData!G29*1.5</f>
+        <v>217.5</v>
+      </c>
+      <c r="H29" s="1">
+        <f>MonsterBaseData!H29</f>
+        <v>1.175</v>
+      </c>
+      <c r="I29" s="1">
+        <f>MonsterBaseData!I29</f>
+        <v>1.65</v>
+      </c>
+      <c r="J29" s="1">
+        <f>MonsterBaseData!J29*1.5</f>
+        <v>55.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
+        <f>MonsterBaseData!A30</f>
+        <v>29</v>
+      </c>
+      <c r="C30" s="1"/>
+      <c r="D30" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E30" s="1">
+        <f>MonsterBaseData!E30</f>
+        <v>29</v>
+      </c>
+      <c r="F30" s="1">
+        <f>MonsterBaseData!F30</f>
+        <v>150</v>
+      </c>
+      <c r="G30" s="1">
+        <f>MonsterBaseData!G30*1.5</f>
+        <v>225</v>
+      </c>
+      <c r="H30" s="1">
+        <f>MonsterBaseData!H30</f>
+        <v>1.2</v>
+      </c>
+      <c r="I30" s="1">
+        <f>MonsterBaseData!I30</f>
+        <v>1.7</v>
+      </c>
+      <c r="J30" s="1">
+        <f>MonsterBaseData!J30*1.5</f>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
+        <f>MonsterBaseData!A31</f>
+        <v>30</v>
+      </c>
+      <c r="C31" s="1"/>
+      <c r="D31" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E31" s="1">
+        <f>MonsterBaseData!E31</f>
+        <v>30</v>
+      </c>
+      <c r="F31" s="1">
+        <f>MonsterBaseData!F31</f>
+        <v>155</v>
+      </c>
+      <c r="G31" s="1">
+        <f>MonsterBaseData!G31*1.5</f>
+        <v>232.5</v>
+      </c>
+      <c r="H31" s="1">
+        <f>MonsterBaseData!H31</f>
+        <v>1.2250000000000001</v>
+      </c>
+      <c r="I31" s="1">
+        <f>MonsterBaseData!I31</f>
+        <v>1.75</v>
+      </c>
+      <c r="J31" s="1">
+        <f>MonsterBaseData!J31*1.5</f>
+        <v>58.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A32" s="1">
+        <f>MonsterBaseData!A32</f>
+        <v>31</v>
+      </c>
+      <c r="C32" s="1"/>
+      <c r="D32" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E32" s="1">
+        <f>MonsterBaseData!E32</f>
+        <v>31</v>
+      </c>
+      <c r="F32" s="1">
+        <f>MonsterBaseData!F32</f>
+        <v>160</v>
+      </c>
+      <c r="G32" s="1">
+        <f>MonsterBaseData!G32*1.5</f>
+        <v>240</v>
+      </c>
+      <c r="H32" s="1">
+        <f>MonsterBaseData!H32</f>
+        <v>1.25</v>
+      </c>
+      <c r="I32" s="1">
+        <f>MonsterBaseData!I32</f>
+        <v>1.8</v>
+      </c>
+      <c r="J32" s="1">
+        <f>MonsterBaseData!J32*1.5</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A33" s="1">
+        <f>MonsterBaseData!A33</f>
+        <v>32</v>
+      </c>
+      <c r="C33" s="1"/>
+      <c r="D33" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E33" s="1">
+        <f>MonsterBaseData!E33</f>
+        <v>32</v>
+      </c>
+      <c r="F33" s="1">
+        <f>MonsterBaseData!F33</f>
+        <v>165</v>
+      </c>
+      <c r="G33" s="1">
+        <f>MonsterBaseData!G33*1.5</f>
+        <v>247.5</v>
+      </c>
+      <c r="H33" s="1">
+        <f>MonsterBaseData!H33</f>
+        <v>1.2749999999999999</v>
+      </c>
+      <c r="I33" s="1">
+        <f>MonsterBaseData!I33</f>
+        <v>1.85</v>
+      </c>
+      <c r="J33" s="1">
+        <f>MonsterBaseData!J33*1.5</f>
+        <v>61.5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A34" s="1">
+        <f>MonsterBaseData!A34</f>
+        <v>33</v>
+      </c>
+      <c r="C34" s="1"/>
+      <c r="D34" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E34" s="1">
+        <f>MonsterBaseData!E34</f>
+        <v>33</v>
+      </c>
+      <c r="F34" s="1">
+        <f>MonsterBaseData!F34</f>
+        <v>170</v>
+      </c>
+      <c r="G34" s="1">
+        <f>MonsterBaseData!G34*1.5</f>
+        <v>255</v>
+      </c>
+      <c r="H34" s="1">
+        <f>MonsterBaseData!H34</f>
+        <v>1.3</v>
+      </c>
+      <c r="I34" s="1">
+        <f>MonsterBaseData!I34</f>
+        <v>1.9</v>
+      </c>
+      <c r="J34" s="1">
+        <f>MonsterBaseData!J34*1.5</f>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A35" s="1">
+        <f>MonsterBaseData!A35</f>
+        <v>34</v>
+      </c>
+      <c r="C35" s="1"/>
+      <c r="D35" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E35" s="1">
+        <f>MonsterBaseData!E35</f>
+        <v>34</v>
+      </c>
+      <c r="F35" s="1">
+        <f>MonsterBaseData!F35</f>
+        <v>175</v>
+      </c>
+      <c r="G35" s="1">
+        <f>MonsterBaseData!G35*1.5</f>
+        <v>262.5</v>
+      </c>
+      <c r="H35" s="1">
+        <f>MonsterBaseData!H35</f>
+        <v>1.325</v>
+      </c>
+      <c r="I35" s="1">
+        <f>MonsterBaseData!I35</f>
+        <v>1.95</v>
+      </c>
+      <c r="J35" s="1">
+        <f>MonsterBaseData!J35*1.5</f>
+        <v>64.5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A36" s="1">
+        <f>MonsterBaseData!A36</f>
+        <v>35</v>
+      </c>
+      <c r="C36" s="1"/>
+      <c r="D36" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E36" s="1">
+        <f>MonsterBaseData!E36</f>
+        <v>35</v>
+      </c>
+      <c r="F36" s="1">
+        <f>MonsterBaseData!F36</f>
+        <v>180</v>
+      </c>
+      <c r="G36" s="1">
+        <f>MonsterBaseData!G36*1.5</f>
+        <v>270</v>
+      </c>
+      <c r="H36" s="1">
+        <f>MonsterBaseData!H36</f>
+        <v>1.35</v>
+      </c>
+      <c r="I36" s="1">
+        <f>MonsterBaseData!I36</f>
+        <v>2</v>
+      </c>
+      <c r="J36" s="1">
+        <f>MonsterBaseData!J36*1.5</f>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A37" s="1">
+        <f>MonsterBaseData!A37</f>
+        <v>36</v>
+      </c>
+      <c r="C37" s="1"/>
+      <c r="D37" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E37" s="1">
+        <f>MonsterBaseData!E37</f>
+        <v>36</v>
+      </c>
+      <c r="F37" s="1">
+        <f>MonsterBaseData!F37</f>
+        <v>185</v>
+      </c>
+      <c r="G37" s="1">
+        <f>MonsterBaseData!G37*1.5</f>
+        <v>277.5</v>
+      </c>
+      <c r="H37" s="1">
+        <f>MonsterBaseData!H37</f>
+        <v>1.375</v>
+      </c>
+      <c r="I37" s="1">
+        <f>MonsterBaseData!I37</f>
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="J37" s="1">
+        <f>MonsterBaseData!J37*1.5</f>
+        <v>67.5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A38" s="1">
+        <f>MonsterBaseData!A38</f>
+        <v>37</v>
+      </c>
+      <c r="C38" s="1"/>
+      <c r="D38" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E38" s="1">
+        <f>MonsterBaseData!E38</f>
+        <v>37</v>
+      </c>
+      <c r="F38" s="1">
+        <f>MonsterBaseData!F38</f>
+        <v>190</v>
+      </c>
+      <c r="G38" s="1">
+        <f>MonsterBaseData!G38*1.5</f>
+        <v>285</v>
+      </c>
+      <c r="H38" s="1">
+        <f>MonsterBaseData!H38</f>
+        <v>1.4</v>
+      </c>
+      <c r="I38" s="1">
+        <f>MonsterBaseData!I38</f>
+        <v>2.1</v>
+      </c>
+      <c r="J38" s="1">
+        <f>MonsterBaseData!J38*1.5</f>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A39" s="1">
+        <f>MonsterBaseData!A39</f>
+        <v>38</v>
+      </c>
+      <c r="C39" s="1"/>
+      <c r="D39" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E39" s="1">
+        <f>MonsterBaseData!E39</f>
+        <v>38</v>
+      </c>
+      <c r="F39" s="1">
+        <f>MonsterBaseData!F39</f>
+        <v>195</v>
+      </c>
+      <c r="G39" s="1">
+        <f>MonsterBaseData!G39*1.5</f>
+        <v>292.5</v>
+      </c>
+      <c r="H39" s="1">
+        <f>MonsterBaseData!H39</f>
+        <v>1.425</v>
+      </c>
+      <c r="I39" s="1">
+        <f>MonsterBaseData!I39</f>
+        <v>2.15</v>
+      </c>
+      <c r="J39" s="1">
+        <f>MonsterBaseData!J39*1.5</f>
+        <v>70.5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A40" s="1">
+        <f>MonsterBaseData!A40</f>
+        <v>39</v>
+      </c>
+      <c r="C40" s="1"/>
+      <c r="D40" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E40" s="1">
+        <f>MonsterBaseData!E40</f>
+        <v>39</v>
+      </c>
+      <c r="F40" s="1">
+        <f>MonsterBaseData!F40</f>
+        <v>200</v>
+      </c>
+      <c r="G40" s="1">
+        <f>MonsterBaseData!G40*1.5</f>
+        <v>300</v>
+      </c>
+      <c r="H40" s="1">
+        <f>MonsterBaseData!H40</f>
+        <v>1.45</v>
+      </c>
+      <c r="I40" s="1">
+        <f>MonsterBaseData!I40</f>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="J40" s="1">
+        <f>MonsterBaseData!J40*1.5</f>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C41" s="1"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C42" s="1"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C43" s="1"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C44" s="1"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C45" s="1"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C46" s="1"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C47" s="1"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C48" s="1"/>
+    </row>
+    <row r="49" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C49" s="1"/>
+    </row>
+    <row r="50" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C50" s="1"/>
+    </row>
+    <row r="51" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C51" s="1"/>
+    </row>
+    <row r="52" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C52" s="1"/>
+    </row>
+    <row r="53" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C53" s="1"/>
+    </row>
+    <row r="54" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C54" s="1"/>
+    </row>
+    <row r="55" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C55" s="1"/>
+    </row>
+    <row r="56" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C56" s="1"/>
+    </row>
+    <row r="57" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C57" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3521,7 +4916,7 @@
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576" xr:uid="{3F7F906E-6C9A-4B61-8B66-8773D370EC07}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B58:B1048576" xr:uid="{3F7F906E-6C9A-4B61-8B66-8773D370EC07}">
       <formula1>$L$2:$L$962</formula1>
     </dataValidation>
   </dataValidations>
@@ -3535,10 +4930,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F360BF2-F57C-43E4-A45B-98C9530388AF}">
-  <dimension ref="A1:K14"/>
+  <dimension ref="A1:K40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3546,13 +4941,13 @@
     <col min="1" max="1" width="6.125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.75" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.375" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.5" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.5" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20.125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17.5" style="1" customWidth="1"/>
-    <col min="10" max="10" width="9.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.75" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="32.875" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="16384" width="9" style="1"/>
   </cols>
@@ -3562,28 +4957,31 @@
         <v>3</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
+      <c r="D1" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="E1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>4</v>
+      <c r="J1" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>0</v>
@@ -3591,102 +4989,1334 @@
     </row>
     <row r="2" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
+        <f>MonsterBaseData!A2</f>
         <v>1</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="J2" s="6"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="1">
+        <f>MonsterBaseData!E2</f>
+        <v>1</v>
+      </c>
+      <c r="F2" s="1">
+        <f>MonsterBaseData!F2</f>
+        <v>10</v>
+      </c>
+      <c r="G2" s="1">
+        <f>MonsterBaseData!G2*0.5</f>
+        <v>5</v>
+      </c>
+      <c r="H2" s="1">
+        <f>MonsterBaseData!H2</f>
+        <v>0.5</v>
+      </c>
+      <c r="I2" s="1">
+        <f>MonsterBaseData!I2*1.5</f>
+        <v>0.44999999999999996</v>
+      </c>
+      <c r="J2" s="1">
+        <f>MonsterBaseData!J2</f>
+        <v>10</v>
+      </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
+        <f>MonsterBaseData!A3</f>
         <v>2</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="J3" s="6"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="1">
+        <f>MonsterBaseData!E3</f>
+        <v>2</v>
+      </c>
+      <c r="F3" s="1">
+        <f>MonsterBaseData!F3</f>
+        <v>15</v>
+      </c>
+      <c r="G3" s="1">
+        <f>MonsterBaseData!G3*0.5</f>
+        <v>7.5</v>
+      </c>
+      <c r="H3" s="1">
+        <f>MonsterBaseData!H3</f>
+        <v>0.52500000000000002</v>
+      </c>
+      <c r="I3" s="1">
+        <f>MonsterBaseData!I3*1.5</f>
+        <v>0.52499999999999991</v>
+      </c>
+      <c r="J3" s="1">
+        <f>MonsterBaseData!J3</f>
+        <v>11</v>
+      </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
+        <f>MonsterBaseData!A4</f>
         <v>3</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="J4" s="6"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="1">
+        <f>MonsterBaseData!E4</f>
+        <v>3</v>
+      </c>
+      <c r="F4" s="1">
+        <f>MonsterBaseData!F4</f>
+        <v>20</v>
+      </c>
+      <c r="G4" s="1">
+        <f>MonsterBaseData!G4*0.5</f>
+        <v>10</v>
+      </c>
+      <c r="H4" s="1">
+        <f>MonsterBaseData!H4</f>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="I4" s="1">
+        <f>MonsterBaseData!I4*1.5</f>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="J4" s="1">
+        <f>MonsterBaseData!J4</f>
+        <v>12</v>
+      </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
+        <f>MonsterBaseData!A5</f>
         <v>4</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="J5" s="6"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="1">
+        <f>MonsterBaseData!E5</f>
+        <v>4</v>
+      </c>
+      <c r="F5" s="1">
+        <f>MonsterBaseData!F5</f>
+        <v>25</v>
+      </c>
+      <c r="G5" s="1">
+        <f>MonsterBaseData!G5*0.5</f>
+        <v>12.5</v>
+      </c>
+      <c r="H5" s="1">
+        <f>MonsterBaseData!H5</f>
+        <v>0.57499999999999996</v>
+      </c>
+      <c r="I5" s="1">
+        <f>MonsterBaseData!I5*1.5</f>
+        <v>0.67500000000000004</v>
+      </c>
+      <c r="J5" s="1">
+        <f>MonsterBaseData!J5</f>
+        <v>13</v>
+      </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
+        <f>MonsterBaseData!A6</f>
         <v>5</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="J6" s="6"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="1">
+        <f>MonsterBaseData!E6</f>
+        <v>5</v>
+      </c>
+      <c r="F6" s="1">
+        <f>MonsterBaseData!F6</f>
+        <v>30</v>
+      </c>
+      <c r="G6" s="1">
+        <f>MonsterBaseData!G6*0.5</f>
+        <v>15</v>
+      </c>
+      <c r="H6" s="1">
+        <f>MonsterBaseData!H6</f>
+        <v>0.6</v>
+      </c>
+      <c r="I6" s="1">
+        <f>MonsterBaseData!I6*1.5</f>
+        <v>0.75</v>
+      </c>
+      <c r="J6" s="1">
+        <f>MonsterBaseData!J6</f>
+        <v>14</v>
+      </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
+        <f>MonsterBaseData!A7</f>
         <v>6</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="J7" s="6"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="1">
+        <f>MonsterBaseData!E7</f>
+        <v>6</v>
+      </c>
+      <c r="F7" s="1">
+        <f>MonsterBaseData!F7</f>
+        <v>35</v>
+      </c>
+      <c r="G7" s="1">
+        <f>MonsterBaseData!G7*0.5</f>
+        <v>17.5</v>
+      </c>
+      <c r="H7" s="1">
+        <f>MonsterBaseData!H7</f>
+        <v>0.625</v>
+      </c>
+      <c r="I7" s="1">
+        <f>MonsterBaseData!I7*1.5</f>
+        <v>0.82500000000000007</v>
+      </c>
+      <c r="J7" s="1">
+        <f>MonsterBaseData!J7</f>
+        <v>15</v>
+      </c>
     </row>
     <row r="8" spans="1:11" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
+        <f>MonsterBaseData!A8</f>
         <v>7</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="J8" s="6"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="1">
+        <f>MonsterBaseData!E8</f>
+        <v>7</v>
+      </c>
+      <c r="F8" s="1">
+        <f>MonsterBaseData!F8</f>
+        <v>40</v>
+      </c>
+      <c r="G8" s="1">
+        <f>MonsterBaseData!G8*0.5</f>
+        <v>20</v>
+      </c>
+      <c r="H8" s="1">
+        <f>MonsterBaseData!H8</f>
+        <v>0.65</v>
+      </c>
+      <c r="I8" s="1">
+        <f>MonsterBaseData!I8*1.5</f>
+        <v>0.89999999999999991</v>
+      </c>
+      <c r="J8" s="1">
+        <f>MonsterBaseData!J8</f>
+        <v>16</v>
+      </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
+        <f>MonsterBaseData!A9</f>
         <v>8</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="J9" s="7"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="1">
+        <f>MonsterBaseData!E9</f>
+        <v>8</v>
+      </c>
+      <c r="F9" s="1">
+        <f>MonsterBaseData!F9</f>
+        <v>45</v>
+      </c>
+      <c r="G9" s="1">
+        <f>MonsterBaseData!G9*0.5</f>
+        <v>22.5</v>
+      </c>
+      <c r="H9" s="1">
+        <f>MonsterBaseData!H9</f>
+        <v>0.67500000000000004</v>
+      </c>
+      <c r="I9" s="1">
+        <f>MonsterBaseData!I9*1.5</f>
+        <v>0.97500000000000009</v>
+      </c>
+      <c r="J9" s="1">
+        <f>MonsterBaseData!J9</f>
+        <v>17</v>
+      </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
+        <f>MonsterBaseData!A10</f>
         <v>9</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="J10" s="7"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="1">
+        <f>MonsterBaseData!E10</f>
+        <v>9</v>
+      </c>
+      <c r="F10" s="1">
+        <f>MonsterBaseData!F10</f>
+        <v>50</v>
+      </c>
+      <c r="G10" s="1">
+        <f>MonsterBaseData!G10*0.5</f>
+        <v>25</v>
+      </c>
+      <c r="H10" s="1">
+        <f>MonsterBaseData!H10</f>
+        <v>0.7</v>
+      </c>
+      <c r="I10" s="1">
+        <f>MonsterBaseData!I10*1.5</f>
+        <v>1.0499999999999998</v>
+      </c>
+      <c r="J10" s="1">
+        <f>MonsterBaseData!J10</f>
+        <v>18</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
+        <f>MonsterBaseData!A11</f>
         <v>10</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="J11" s="7"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="1">
+        <f>MonsterBaseData!E11</f>
+        <v>10</v>
+      </c>
+      <c r="F11" s="1">
+        <f>MonsterBaseData!F11</f>
+        <v>55</v>
+      </c>
+      <c r="G11" s="1">
+        <f>MonsterBaseData!G11*0.5</f>
+        <v>27.5</v>
+      </c>
+      <c r="H11" s="1">
+        <f>MonsterBaseData!H11</f>
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="I11" s="1">
+        <f>MonsterBaseData!I11*1.5</f>
+        <v>1.125</v>
+      </c>
+      <c r="J11" s="1">
+        <f>MonsterBaseData!J11</f>
+        <v>19</v>
+      </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
+        <f>MonsterBaseData!A12</f>
         <v>11</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="J12" s="7"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="1">
+        <f>MonsterBaseData!E12</f>
+        <v>11</v>
+      </c>
+      <c r="F12" s="1">
+        <f>MonsterBaseData!F12</f>
+        <v>60</v>
+      </c>
+      <c r="G12" s="1">
+        <f>MonsterBaseData!G12*0.5</f>
+        <v>30</v>
+      </c>
+      <c r="H12" s="1">
+        <f>MonsterBaseData!H12</f>
+        <v>0.75</v>
+      </c>
+      <c r="I12" s="1">
+        <f>MonsterBaseData!I12*1.5</f>
+        <v>1.2000000000000002</v>
+      </c>
+      <c r="J12" s="1">
+        <f>MonsterBaseData!J12</f>
+        <v>20</v>
+      </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
+        <f>MonsterBaseData!A13</f>
         <v>12</v>
       </c>
-      <c r="C13" s="4"/>
-      <c r="J13" s="7"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="1">
+        <f>MonsterBaseData!E13</f>
+        <v>12</v>
+      </c>
+      <c r="F13" s="1">
+        <f>MonsterBaseData!F13</f>
+        <v>65</v>
+      </c>
+      <c r="G13" s="1">
+        <f>MonsterBaseData!G13*0.5</f>
+        <v>32.5</v>
+      </c>
+      <c r="H13" s="1">
+        <f>MonsterBaseData!H13</f>
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="I13" s="1">
+        <f>MonsterBaseData!I13*1.5</f>
+        <v>1.2749999999999999</v>
+      </c>
+      <c r="J13" s="1">
+        <f>MonsterBaseData!J13</f>
+        <v>21</v>
+      </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
+        <f>MonsterBaseData!A14</f>
         <v>13</v>
       </c>
-      <c r="C14" s="4"/>
-      <c r="J14" s="7"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="1">
+        <f>MonsterBaseData!E14</f>
+        <v>13</v>
+      </c>
+      <c r="F14" s="1">
+        <f>MonsterBaseData!F14</f>
+        <v>70</v>
+      </c>
+      <c r="G14" s="1">
+        <f>MonsterBaseData!G14*0.5</f>
+        <v>35</v>
+      </c>
+      <c r="H14" s="1">
+        <f>MonsterBaseData!H14</f>
+        <v>0.8</v>
+      </c>
+      <c r="I14" s="1">
+        <f>MonsterBaseData!I14*1.5</f>
+        <v>1.35</v>
+      </c>
+      <c r="J14" s="1">
+        <f>MonsterBaseData!J14</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <f>MonsterBaseData!A15</f>
+        <v>14</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="D15" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" s="1">
+        <f>MonsterBaseData!E15</f>
+        <v>14</v>
+      </c>
+      <c r="F15" s="1">
+        <f>MonsterBaseData!F15</f>
+        <v>75</v>
+      </c>
+      <c r="G15" s="1">
+        <f>MonsterBaseData!G15*0.5</f>
+        <v>37.5</v>
+      </c>
+      <c r="H15" s="1">
+        <f>MonsterBaseData!H15</f>
+        <v>0.82499999999999996</v>
+      </c>
+      <c r="I15" s="1">
+        <f>MonsterBaseData!I15*1.5</f>
+        <v>1.4249999999999998</v>
+      </c>
+      <c r="J15" s="1">
+        <f>MonsterBaseData!J15</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <f>MonsterBaseData!A16</f>
+        <v>15</v>
+      </c>
+      <c r="C16" s="1"/>
+      <c r="D16" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" s="1">
+        <f>MonsterBaseData!E16</f>
+        <v>15</v>
+      </c>
+      <c r="F16" s="1">
+        <f>MonsterBaseData!F16</f>
+        <v>80</v>
+      </c>
+      <c r="G16" s="1">
+        <f>MonsterBaseData!G16*0.5</f>
+        <v>40</v>
+      </c>
+      <c r="H16" s="1">
+        <f>MonsterBaseData!H16</f>
+        <v>0.85</v>
+      </c>
+      <c r="I16" s="1">
+        <f>MonsterBaseData!I16*1.5</f>
+        <v>1.5</v>
+      </c>
+      <c r="J16" s="1">
+        <f>MonsterBaseData!J16</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <f>MonsterBaseData!A17</f>
+        <v>16</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="D17" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" s="1">
+        <f>MonsterBaseData!E17</f>
+        <v>16</v>
+      </c>
+      <c r="F17" s="1">
+        <f>MonsterBaseData!F17</f>
+        <v>85</v>
+      </c>
+      <c r="G17" s="1">
+        <f>MonsterBaseData!G17*0.5</f>
+        <v>42.5</v>
+      </c>
+      <c r="H17" s="1">
+        <f>MonsterBaseData!H17</f>
+        <v>0.875</v>
+      </c>
+      <c r="I17" s="1">
+        <f>MonsterBaseData!I17*1.5</f>
+        <v>1.5750000000000002</v>
+      </c>
+      <c r="J17" s="1">
+        <f>MonsterBaseData!J17</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <f>MonsterBaseData!A18</f>
+        <v>17</v>
+      </c>
+      <c r="C18" s="1"/>
+      <c r="D18" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" s="1">
+        <f>MonsterBaseData!E18</f>
+        <v>17</v>
+      </c>
+      <c r="F18" s="1">
+        <f>MonsterBaseData!F18</f>
+        <v>90</v>
+      </c>
+      <c r="G18" s="1">
+        <f>MonsterBaseData!G18*0.5</f>
+        <v>45</v>
+      </c>
+      <c r="H18" s="1">
+        <f>MonsterBaseData!H18</f>
+        <v>0.9</v>
+      </c>
+      <c r="I18" s="1">
+        <f>MonsterBaseData!I18*1.5</f>
+        <v>1.6500000000000001</v>
+      </c>
+      <c r="J18" s="1">
+        <f>MonsterBaseData!J18</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <f>MonsterBaseData!A19</f>
+        <v>18</v>
+      </c>
+      <c r="C19" s="1"/>
+      <c r="D19" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19" s="1">
+        <f>MonsterBaseData!E19</f>
+        <v>18</v>
+      </c>
+      <c r="F19" s="1">
+        <f>MonsterBaseData!F19</f>
+        <v>95</v>
+      </c>
+      <c r="G19" s="1">
+        <f>MonsterBaseData!G19*0.5</f>
+        <v>47.5</v>
+      </c>
+      <c r="H19" s="1">
+        <f>MonsterBaseData!H19</f>
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="I19" s="1">
+        <f>MonsterBaseData!I19*1.5</f>
+        <v>1.7249999999999999</v>
+      </c>
+      <c r="J19" s="1">
+        <f>MonsterBaseData!J19</f>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <f>MonsterBaseData!A20</f>
+        <v>19</v>
+      </c>
+      <c r="C20" s="1"/>
+      <c r="D20" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20" s="1">
+        <f>MonsterBaseData!E20</f>
+        <v>19</v>
+      </c>
+      <c r="F20" s="1">
+        <f>MonsterBaseData!F20</f>
+        <v>100</v>
+      </c>
+      <c r="G20" s="1">
+        <f>MonsterBaseData!G20*0.5</f>
+        <v>50</v>
+      </c>
+      <c r="H20" s="1">
+        <f>MonsterBaseData!H20</f>
+        <v>0.95</v>
+      </c>
+      <c r="I20" s="1">
+        <f>MonsterBaseData!I20*1.5</f>
+        <v>1.7999999999999998</v>
+      </c>
+      <c r="J20" s="1">
+        <f>MonsterBaseData!J20</f>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <f>MonsterBaseData!A21</f>
+        <v>20</v>
+      </c>
+      <c r="C21" s="1"/>
+      <c r="D21" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" s="1">
+        <f>MonsterBaseData!E21</f>
+        <v>20</v>
+      </c>
+      <c r="F21" s="1">
+        <f>MonsterBaseData!F21</f>
+        <v>105</v>
+      </c>
+      <c r="G21" s="1">
+        <f>MonsterBaseData!G21*0.5</f>
+        <v>52.5</v>
+      </c>
+      <c r="H21" s="1">
+        <f>MonsterBaseData!H21</f>
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="I21" s="1">
+        <f>MonsterBaseData!I21*1.5</f>
+        <v>1.875</v>
+      </c>
+      <c r="J21" s="1">
+        <f>MonsterBaseData!J21</f>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <f>MonsterBaseData!A22</f>
+        <v>21</v>
+      </c>
+      <c r="C22" s="1"/>
+      <c r="D22" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E22" s="1">
+        <f>MonsterBaseData!E22</f>
+        <v>21</v>
+      </c>
+      <c r="F22" s="1">
+        <f>MonsterBaseData!F22</f>
+        <v>110</v>
+      </c>
+      <c r="G22" s="1">
+        <f>MonsterBaseData!G22*0.5</f>
+        <v>55</v>
+      </c>
+      <c r="H22" s="1">
+        <f>MonsterBaseData!H22</f>
+        <v>1</v>
+      </c>
+      <c r="I22" s="1">
+        <f>MonsterBaseData!I22*1.5</f>
+        <v>1.9500000000000002</v>
+      </c>
+      <c r="J22" s="1">
+        <f>MonsterBaseData!J22</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <f>MonsterBaseData!A23</f>
+        <v>22</v>
+      </c>
+      <c r="C23" s="1"/>
+      <c r="D23" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23" s="1">
+        <f>MonsterBaseData!E23</f>
+        <v>22</v>
+      </c>
+      <c r="F23" s="1">
+        <f>MonsterBaseData!F23</f>
+        <v>115</v>
+      </c>
+      <c r="G23" s="1">
+        <f>MonsterBaseData!G23*0.5</f>
+        <v>57.5</v>
+      </c>
+      <c r="H23" s="1">
+        <f>MonsterBaseData!H23</f>
+        <v>1.0249999999999999</v>
+      </c>
+      <c r="I23" s="1">
+        <f>MonsterBaseData!I23*1.5</f>
+        <v>2.0250000000000004</v>
+      </c>
+      <c r="J23" s="1">
+        <f>MonsterBaseData!J23</f>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <f>MonsterBaseData!A24</f>
+        <v>23</v>
+      </c>
+      <c r="C24" s="1"/>
+      <c r="D24" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E24" s="1">
+        <f>MonsterBaseData!E24</f>
+        <v>23</v>
+      </c>
+      <c r="F24" s="1">
+        <f>MonsterBaseData!F24</f>
+        <v>120</v>
+      </c>
+      <c r="G24" s="1">
+        <f>MonsterBaseData!G24*0.5</f>
+        <v>60</v>
+      </c>
+      <c r="H24" s="1">
+        <f>MonsterBaseData!H24</f>
+        <v>1.05</v>
+      </c>
+      <c r="I24" s="1">
+        <f>MonsterBaseData!I24*1.5</f>
+        <v>2.0999999999999996</v>
+      </c>
+      <c r="J24" s="1">
+        <f>MonsterBaseData!J24</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <f>MonsterBaseData!A25</f>
+        <v>24</v>
+      </c>
+      <c r="C25" s="1"/>
+      <c r="D25" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E25" s="1">
+        <f>MonsterBaseData!E25</f>
+        <v>24</v>
+      </c>
+      <c r="F25" s="1">
+        <f>MonsterBaseData!F25</f>
+        <v>125</v>
+      </c>
+      <c r="G25" s="1">
+        <f>MonsterBaseData!G25*0.5</f>
+        <v>62.5</v>
+      </c>
+      <c r="H25" s="1">
+        <f>MonsterBaseData!H25</f>
+        <v>1.075</v>
+      </c>
+      <c r="I25" s="1">
+        <f>MonsterBaseData!I25*1.5</f>
+        <v>2.1749999999999998</v>
+      </c>
+      <c r="J25" s="1">
+        <f>MonsterBaseData!J25</f>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
+        <f>MonsterBaseData!A26</f>
+        <v>25</v>
+      </c>
+      <c r="C26" s="1"/>
+      <c r="D26" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E26" s="1">
+        <f>MonsterBaseData!E26</f>
+        <v>25</v>
+      </c>
+      <c r="F26" s="1">
+        <f>MonsterBaseData!F26</f>
+        <v>130</v>
+      </c>
+      <c r="G26" s="1">
+        <f>MonsterBaseData!G26*0.5</f>
+        <v>65</v>
+      </c>
+      <c r="H26" s="1">
+        <f>MonsterBaseData!H26</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="I26" s="1">
+        <f>MonsterBaseData!I26*1.5</f>
+        <v>2.25</v>
+      </c>
+      <c r="J26" s="1">
+        <f>MonsterBaseData!J26</f>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <f>MonsterBaseData!A27</f>
+        <v>26</v>
+      </c>
+      <c r="C27" s="1"/>
+      <c r="D27" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E27" s="1">
+        <f>MonsterBaseData!E27</f>
+        <v>26</v>
+      </c>
+      <c r="F27" s="1">
+        <f>MonsterBaseData!F27</f>
+        <v>135</v>
+      </c>
+      <c r="G27" s="1">
+        <f>MonsterBaseData!G27*0.5</f>
+        <v>67.5</v>
+      </c>
+      <c r="H27" s="1">
+        <f>MonsterBaseData!H27</f>
+        <v>1.125</v>
+      </c>
+      <c r="I27" s="1">
+        <f>MonsterBaseData!I27*1.5</f>
+        <v>2.3250000000000002</v>
+      </c>
+      <c r="J27" s="1">
+        <f>MonsterBaseData!J27</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
+        <f>MonsterBaseData!A28</f>
+        <v>27</v>
+      </c>
+      <c r="C28" s="1"/>
+      <c r="D28" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E28" s="1">
+        <f>MonsterBaseData!E28</f>
+        <v>27</v>
+      </c>
+      <c r="F28" s="1">
+        <f>MonsterBaseData!F28</f>
+        <v>140</v>
+      </c>
+      <c r="G28" s="1">
+        <f>MonsterBaseData!G28*0.5</f>
+        <v>70</v>
+      </c>
+      <c r="H28" s="1">
+        <f>MonsterBaseData!H28</f>
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="I28" s="1">
+        <f>MonsterBaseData!I28*1.5</f>
+        <v>2.4000000000000004</v>
+      </c>
+      <c r="J28" s="1">
+        <f>MonsterBaseData!J28</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
+        <f>MonsterBaseData!A29</f>
+        <v>28</v>
+      </c>
+      <c r="C29" s="1"/>
+      <c r="D29" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E29" s="1">
+        <f>MonsterBaseData!E29</f>
+        <v>28</v>
+      </c>
+      <c r="F29" s="1">
+        <f>MonsterBaseData!F29</f>
+        <v>145</v>
+      </c>
+      <c r="G29" s="1">
+        <f>MonsterBaseData!G29*0.5</f>
+        <v>72.5</v>
+      </c>
+      <c r="H29" s="1">
+        <f>MonsterBaseData!H29</f>
+        <v>1.175</v>
+      </c>
+      <c r="I29" s="1">
+        <f>MonsterBaseData!I29*1.5</f>
+        <v>2.4749999999999996</v>
+      </c>
+      <c r="J29" s="1">
+        <f>MonsterBaseData!J29</f>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
+        <f>MonsterBaseData!A30</f>
+        <v>29</v>
+      </c>
+      <c r="C30" s="1"/>
+      <c r="D30" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E30" s="1">
+        <f>MonsterBaseData!E30</f>
+        <v>29</v>
+      </c>
+      <c r="F30" s="1">
+        <f>MonsterBaseData!F30</f>
+        <v>150</v>
+      </c>
+      <c r="G30" s="1">
+        <f>MonsterBaseData!G30*0.5</f>
+        <v>75</v>
+      </c>
+      <c r="H30" s="1">
+        <f>MonsterBaseData!H30</f>
+        <v>1.2</v>
+      </c>
+      <c r="I30" s="1">
+        <f>MonsterBaseData!I30*1.5</f>
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="J30" s="1">
+        <f>MonsterBaseData!J30</f>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
+        <f>MonsterBaseData!A31</f>
+        <v>30</v>
+      </c>
+      <c r="C31" s="1"/>
+      <c r="D31" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E31" s="1">
+        <f>MonsterBaseData!E31</f>
+        <v>30</v>
+      </c>
+      <c r="F31" s="1">
+        <f>MonsterBaseData!F31</f>
+        <v>155</v>
+      </c>
+      <c r="G31" s="1">
+        <f>MonsterBaseData!G31*0.5</f>
+        <v>77.5</v>
+      </c>
+      <c r="H31" s="1">
+        <f>MonsterBaseData!H31</f>
+        <v>1.2250000000000001</v>
+      </c>
+      <c r="I31" s="1">
+        <f>MonsterBaseData!I31*1.5</f>
+        <v>2.625</v>
+      </c>
+      <c r="J31" s="1">
+        <f>MonsterBaseData!J31</f>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A32" s="1">
+        <f>MonsterBaseData!A32</f>
+        <v>31</v>
+      </c>
+      <c r="C32" s="1"/>
+      <c r="D32" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E32" s="1">
+        <f>MonsterBaseData!E32</f>
+        <v>31</v>
+      </c>
+      <c r="F32" s="1">
+        <f>MonsterBaseData!F32</f>
+        <v>160</v>
+      </c>
+      <c r="G32" s="1">
+        <f>MonsterBaseData!G32*0.5</f>
+        <v>80</v>
+      </c>
+      <c r="H32" s="1">
+        <f>MonsterBaseData!H32</f>
+        <v>1.25</v>
+      </c>
+      <c r="I32" s="1">
+        <f>MonsterBaseData!I32*1.5</f>
+        <v>2.7</v>
+      </c>
+      <c r="J32" s="1">
+        <f>MonsterBaseData!J32</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A33" s="1">
+        <f>MonsterBaseData!A33</f>
+        <v>32</v>
+      </c>
+      <c r="C33" s="1"/>
+      <c r="D33" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E33" s="1">
+        <f>MonsterBaseData!E33</f>
+        <v>32</v>
+      </c>
+      <c r="F33" s="1">
+        <f>MonsterBaseData!F33</f>
+        <v>165</v>
+      </c>
+      <c r="G33" s="1">
+        <f>MonsterBaseData!G33*0.5</f>
+        <v>82.5</v>
+      </c>
+      <c r="H33" s="1">
+        <f>MonsterBaseData!H33</f>
+        <v>1.2749999999999999</v>
+      </c>
+      <c r="I33" s="1">
+        <f>MonsterBaseData!I33*1.5</f>
+        <v>2.7750000000000004</v>
+      </c>
+      <c r="J33" s="1">
+        <f>MonsterBaseData!J33</f>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A34" s="1">
+        <f>MonsterBaseData!A34</f>
+        <v>33</v>
+      </c>
+      <c r="C34" s="1"/>
+      <c r="D34" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E34" s="1">
+        <f>MonsterBaseData!E34</f>
+        <v>33</v>
+      </c>
+      <c r="F34" s="1">
+        <f>MonsterBaseData!F34</f>
+        <v>170</v>
+      </c>
+      <c r="G34" s="1">
+        <f>MonsterBaseData!G34*0.5</f>
+        <v>85</v>
+      </c>
+      <c r="H34" s="1">
+        <f>MonsterBaseData!H34</f>
+        <v>1.3</v>
+      </c>
+      <c r="I34" s="1">
+        <f>MonsterBaseData!I34*1.5</f>
+        <v>2.8499999999999996</v>
+      </c>
+      <c r="J34" s="1">
+        <f>MonsterBaseData!J34</f>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A35" s="1">
+        <f>MonsterBaseData!A35</f>
+        <v>34</v>
+      </c>
+      <c r="C35" s="1"/>
+      <c r="D35" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E35" s="1">
+        <f>MonsterBaseData!E35</f>
+        <v>34</v>
+      </c>
+      <c r="F35" s="1">
+        <f>MonsterBaseData!F35</f>
+        <v>175</v>
+      </c>
+      <c r="G35" s="1">
+        <f>MonsterBaseData!G35*0.5</f>
+        <v>87.5</v>
+      </c>
+      <c r="H35" s="1">
+        <f>MonsterBaseData!H35</f>
+        <v>1.325</v>
+      </c>
+      <c r="I35" s="1">
+        <f>MonsterBaseData!I35*1.5</f>
+        <v>2.9249999999999998</v>
+      </c>
+      <c r="J35" s="1">
+        <f>MonsterBaseData!J35</f>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A36" s="1">
+        <f>MonsterBaseData!A36</f>
+        <v>35</v>
+      </c>
+      <c r="C36" s="1"/>
+      <c r="D36" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E36" s="1">
+        <f>MonsterBaseData!E36</f>
+        <v>35</v>
+      </c>
+      <c r="F36" s="1">
+        <f>MonsterBaseData!F36</f>
+        <v>180</v>
+      </c>
+      <c r="G36" s="1">
+        <f>MonsterBaseData!G36*0.5</f>
+        <v>90</v>
+      </c>
+      <c r="H36" s="1">
+        <f>MonsterBaseData!H36</f>
+        <v>1.35</v>
+      </c>
+      <c r="I36" s="1">
+        <f>MonsterBaseData!I36*1.5</f>
+        <v>3</v>
+      </c>
+      <c r="J36" s="1">
+        <f>MonsterBaseData!J36</f>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A37" s="1">
+        <f>MonsterBaseData!A37</f>
+        <v>36</v>
+      </c>
+      <c r="C37" s="1"/>
+      <c r="D37" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E37" s="1">
+        <f>MonsterBaseData!E37</f>
+        <v>36</v>
+      </c>
+      <c r="F37" s="1">
+        <f>MonsterBaseData!F37</f>
+        <v>185</v>
+      </c>
+      <c r="G37" s="1">
+        <f>MonsterBaseData!G37*0.5</f>
+        <v>92.5</v>
+      </c>
+      <c r="H37" s="1">
+        <f>MonsterBaseData!H37</f>
+        <v>1.375</v>
+      </c>
+      <c r="I37" s="1">
+        <f>MonsterBaseData!I37*1.5</f>
+        <v>3.0749999999999997</v>
+      </c>
+      <c r="J37" s="1">
+        <f>MonsterBaseData!J37</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A38" s="1">
+        <f>MonsterBaseData!A38</f>
+        <v>37</v>
+      </c>
+      <c r="C38" s="1"/>
+      <c r="D38" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E38" s="1">
+        <f>MonsterBaseData!E38</f>
+        <v>37</v>
+      </c>
+      <c r="F38" s="1">
+        <f>MonsterBaseData!F38</f>
+        <v>190</v>
+      </c>
+      <c r="G38" s="1">
+        <f>MonsterBaseData!G38*0.5</f>
+        <v>95</v>
+      </c>
+      <c r="H38" s="1">
+        <f>MonsterBaseData!H38</f>
+        <v>1.4</v>
+      </c>
+      <c r="I38" s="1">
+        <f>MonsterBaseData!I38*1.5</f>
+        <v>3.1500000000000004</v>
+      </c>
+      <c r="J38" s="1">
+        <f>MonsterBaseData!J38</f>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A39" s="1">
+        <f>MonsterBaseData!A39</f>
+        <v>38</v>
+      </c>
+      <c r="C39" s="1"/>
+      <c r="D39" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E39" s="1">
+        <f>MonsterBaseData!E39</f>
+        <v>38</v>
+      </c>
+      <c r="F39" s="1">
+        <f>MonsterBaseData!F39</f>
+        <v>195</v>
+      </c>
+      <c r="G39" s="1">
+        <f>MonsterBaseData!G39*0.5</f>
+        <v>97.5</v>
+      </c>
+      <c r="H39" s="1">
+        <f>MonsterBaseData!H39</f>
+        <v>1.425</v>
+      </c>
+      <c r="I39" s="1">
+        <f>MonsterBaseData!I39*1.5</f>
+        <v>3.2249999999999996</v>
+      </c>
+      <c r="J39" s="1">
+        <f>MonsterBaseData!J39</f>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A40" s="1">
+        <f>MonsterBaseData!A40</f>
+        <v>39</v>
+      </c>
+      <c r="C40" s="1"/>
+      <c r="D40" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E40" s="1">
+        <f>MonsterBaseData!E40</f>
+        <v>39</v>
+      </c>
+      <c r="F40" s="1">
+        <f>MonsterBaseData!F40</f>
+        <v>200</v>
+      </c>
+      <c r="G40" s="1">
+        <f>MonsterBaseData!G40*0.5</f>
+        <v>100</v>
+      </c>
+      <c r="H40" s="1">
+        <f>MonsterBaseData!H40</f>
+        <v>1.45</v>
+      </c>
+      <c r="I40" s="1">
+        <f>MonsterBaseData!I40*1.5</f>
+        <v>3.3000000000000003</v>
+      </c>
+      <c r="J40" s="1">
+        <f>MonsterBaseData!J40</f>
+        <v>48</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="J2:J14"/>
-  </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576" xr:uid="{00A1E1D4-7382-459B-BF8F-8C45AF75A2DE}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B41:B1048576" xr:uid="{00A1E1D4-7382-459B-BF8F-8C45AF75A2DE}">
       <formula1>$K$2:$K$962</formula1>
     </dataValidation>
   </dataValidations>
@@ -3727,7 +6357,7 @@
         <v>3</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
@@ -3736,16 +6366,16 @@
         <v>2</v>
       </c>
       <c r="E1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="5" t="s">
-        <v>8</v>
-      </c>
       <c r="H1" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>4</v>
@@ -3759,91 +6389,91 @@
         <v>1</v>
       </c>
       <c r="C2" s="4"/>
-      <c r="J2" s="6"/>
+      <c r="J2" s="7"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="C3" s="4"/>
-      <c r="J3" s="6"/>
+      <c r="J3" s="7"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="C4" s="4"/>
-      <c r="J4" s="6"/>
+      <c r="J4" s="7"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="C5" s="4"/>
-      <c r="J5" s="6"/>
+      <c r="J5" s="7"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="C6" s="4"/>
-      <c r="J6" s="6"/>
+      <c r="J6" s="7"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="C7" s="4"/>
-      <c r="J7" s="6"/>
+      <c r="J7" s="7"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="C8" s="4"/>
-      <c r="J8" s="6"/>
+      <c r="J8" s="7"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="C9" s="4"/>
-      <c r="J9" s="7"/>
+      <c r="J9" s="8"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="C10" s="4"/>
-      <c r="J10" s="7"/>
+      <c r="J10" s="8"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="C11" s="4"/>
-      <c r="J11" s="7"/>
+      <c r="J11" s="8"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>11</v>
       </c>
       <c r="C12" s="4"/>
-      <c r="J12" s="7"/>
+      <c r="J12" s="8"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>12</v>
       </c>
       <c r="C13" s="4"/>
-      <c r="J13" s="7"/>
+      <c r="J13" s="8"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>13</v>
       </c>
       <c r="C14" s="4"/>
-      <c r="J14" s="7"/>
+      <c r="J14" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
add monster data table category
</commit_message>
<xml_diff>
--- a/Assets/ExcelDataTables/MonsterData.xlsx
+++ b/Assets/ExcelDataTables/MonsterData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UnityProject\UnityKoreaAward\Assets\ExcelDataTables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45C4C3D1-2DD3-4E10-8CC2-E25570AA5E43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7A30FAB-A74F-4573-BE19-14D247E70820}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="16200" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1935" yWindow="765" windowWidth="26505" windowHeight="14565" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MonsterBaseData" sheetId="1" r:id="rId1"/>
@@ -337,7 +337,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -803,7 +803,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{274B8010-E41C-4B84-89D7-C000DBC4CBFF}">
+    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{274B8010-E41C-4B84-89D7-C000DBC4CBFF}">
       <text>
         <r>
           <rPr>
@@ -1269,7 +1269,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{EDE0EC23-3F33-4C7B-8178-0D0A9FAFE577}">
+    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{EDE0EC23-3F33-4C7B-8178-0D0A9FAFE577}">
       <text>
         <r>
           <rPr>
@@ -1859,7 +1859,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="20">
   <si>
     <t>PlayerSkillType DropBox List</t>
   </si>
@@ -1925,6 +1925,14 @@
   </si>
   <si>
     <t>HP::float</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Score::int</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ranged::float</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
@@ -2105,10 +2113,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="표3" displayName="표3" ref="N1:N962" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="N1:N962" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="N962:N1048516">
-    <sortCondition descending="1" ref="N962:N1048516"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="표3" displayName="표3" ref="O1:O962" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="O1:O962" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="O962:O1048516">
+    <sortCondition descending="1" ref="O962:O1048516"/>
   </sortState>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="MonsterSkiilsType DropBox List" dataDxfId="9"/>
@@ -2118,10 +2126,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3E5D2C3E-0D5B-4226-83E1-7737192D74C5}" name="표3_2" displayName="표3_2" ref="L1:L962" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
-  <autoFilter ref="L1:L962" xr:uid="{3E5D2C3E-0D5B-4226-83E1-7737192D74C5}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="L2:L1047556">
-    <sortCondition descending="1" ref="L962:L1048516"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3E5D2C3E-0D5B-4226-83E1-7737192D74C5}" name="표3_2" displayName="표3_2" ref="O1:O962" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="O1:O962" xr:uid="{3E5D2C3E-0D5B-4226-83E1-7737192D74C5}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="O2:O1047556">
+    <sortCondition descending="1" ref="O962:O1048516"/>
   </sortState>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{2FE06BE7-BA42-43F1-B24B-9D4DE22B13AC}" name="PlayerSkillType DropBox List" dataDxfId="6"/>
@@ -2131,10 +2139,10 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{31F112A0-44EC-4418-9C58-159152E7B13B}" name="표3_23" displayName="표3_23" ref="K1:K962" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="K1:K962" xr:uid="{31F112A0-44EC-4418-9C58-159152E7B13B}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="K2:K1047556">
-    <sortCondition descending="1" ref="K962:K1048516"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{31F112A0-44EC-4418-9C58-159152E7B13B}" name="표3_23" displayName="표3_23" ref="N1:N962" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="N1:N962" xr:uid="{31F112A0-44EC-4418-9C58-159152E7B13B}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="N2:N1047556">
+    <sortCondition descending="1" ref="N962:N1048516"/>
   </sortState>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{DAEE0437-F223-4287-AC97-C13E35A555A5}" name="PlayerSkillType DropBox List" dataDxfId="3"/>
@@ -2449,13 +2457,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:N40"/>
+  <dimension ref="A1:O40"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="75" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G2" sqref="G2"/>
+      <selection pane="bottomRight" activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2469,14 +2477,14 @@
     <col min="8" max="8" width="11.5" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.5" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="21.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.25" style="1" customWidth="1"/>
-    <col min="12" max="12" width="17.5" style="1" customWidth="1"/>
-    <col min="13" max="13" width="9.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="30.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9" style="1"/>
+    <col min="11" max="12" width="12.25" style="1" customWidth="1"/>
+    <col min="13" max="13" width="17.5" style="1" customWidth="1"/>
+    <col min="14" max="14" width="9.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="30.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -2507,15 +2515,20 @@
       <c r="J1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2"/>
-      <c r="M1" s="1" t="s">
+      <c r="K1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="O1" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -2538,9 +2551,15 @@
       <c r="J2" s="1">
         <v>10</v>
       </c>
-      <c r="M2" s="7"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="K2" s="1">
+        <v>10</v>
+      </c>
+      <c r="L2" s="1">
+        <v>1</v>
+      </c>
+      <c r="N2" s="7"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -2563,9 +2582,15 @@
       <c r="J3" s="1">
         <v>11</v>
       </c>
-      <c r="M3" s="7"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="K3" s="1">
+        <v>20</v>
+      </c>
+      <c r="L3" s="1">
+        <v>1</v>
+      </c>
+      <c r="N3" s="7"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -2588,9 +2613,15 @@
       <c r="J4" s="1">
         <v>12</v>
       </c>
-      <c r="M4" s="7"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="K4" s="1">
+        <v>30</v>
+      </c>
+      <c r="L4" s="1">
+        <v>1</v>
+      </c>
+      <c r="N4" s="7"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -2613,9 +2644,15 @@
       <c r="J5" s="1">
         <v>13</v>
       </c>
-      <c r="M5" s="7"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="K5" s="1">
+        <v>40</v>
+      </c>
+      <c r="L5" s="1">
+        <v>1</v>
+      </c>
+      <c r="N5" s="7"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -2638,9 +2675,15 @@
       <c r="J6" s="1">
         <v>14</v>
       </c>
-      <c r="M6" s="7"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="K6" s="1">
+        <v>50</v>
+      </c>
+      <c r="L6" s="1">
+        <v>1</v>
+      </c>
+      <c r="N6" s="7"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -2663,9 +2706,15 @@
       <c r="J7" s="1">
         <v>15</v>
       </c>
-      <c r="M7" s="7"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="K7" s="1">
+        <v>60</v>
+      </c>
+      <c r="L7" s="1">
+        <v>1</v>
+      </c>
+      <c r="N7" s="7"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -2688,9 +2737,15 @@
       <c r="J8" s="1">
         <v>16</v>
       </c>
-      <c r="M8" s="7"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="K8" s="1">
+        <v>70</v>
+      </c>
+      <c r="L8" s="1">
+        <v>1</v>
+      </c>
+      <c r="N8" s="7"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -2713,9 +2768,15 @@
       <c r="J9" s="1">
         <v>17</v>
       </c>
-      <c r="M9" s="8"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="K9" s="1">
+        <v>80</v>
+      </c>
+      <c r="L9" s="1">
+        <v>1</v>
+      </c>
+      <c r="N9" s="8"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -2738,9 +2799,15 @@
       <c r="J10" s="1">
         <v>18</v>
       </c>
-      <c r="M10" s="8"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="K10" s="1">
+        <v>90</v>
+      </c>
+      <c r="L10" s="1">
+        <v>1</v>
+      </c>
+      <c r="N10" s="8"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -2763,9 +2830,15 @@
       <c r="J11" s="1">
         <v>19</v>
       </c>
-      <c r="M11" s="8"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="K11" s="1">
+        <v>100</v>
+      </c>
+      <c r="L11" s="1">
+        <v>1</v>
+      </c>
+      <c r="N11" s="8"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -2788,9 +2861,15 @@
       <c r="J12" s="1">
         <v>20</v>
       </c>
-      <c r="M12" s="8"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="K12" s="1">
+        <v>110</v>
+      </c>
+      <c r="L12" s="1">
+        <v>1</v>
+      </c>
+      <c r="N12" s="8"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -2813,9 +2892,15 @@
       <c r="J13" s="1">
         <v>21</v>
       </c>
-      <c r="M13" s="8"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="K13" s="1">
+        <v>120</v>
+      </c>
+      <c r="L13" s="1">
+        <v>1</v>
+      </c>
+      <c r="N13" s="8"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -2838,9 +2923,15 @@
       <c r="J14" s="1">
         <v>22</v>
       </c>
-      <c r="M14" s="8"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="K14" s="1">
+        <v>130</v>
+      </c>
+      <c r="L14" s="1">
+        <v>1</v>
+      </c>
+      <c r="N14" s="8"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -2862,8 +2953,14 @@
       <c r="J15" s="1">
         <v>23</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="K15" s="1">
+        <v>140</v>
+      </c>
+      <c r="L15" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -2885,8 +2982,14 @@
       <c r="J16" s="1">
         <v>24</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K16" s="1">
+        <v>150</v>
+      </c>
+      <c r="L16" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -2908,8 +3011,14 @@
       <c r="J17" s="1">
         <v>25</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K17" s="1">
+        <v>160</v>
+      </c>
+      <c r="L17" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -2931,8 +3040,14 @@
       <c r="J18" s="1">
         <v>26</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K18" s="1">
+        <v>170</v>
+      </c>
+      <c r="L18" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -2954,8 +3069,14 @@
       <c r="J19" s="1">
         <v>27</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K19" s="1">
+        <v>180</v>
+      </c>
+      <c r="L19" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -2977,8 +3098,14 @@
       <c r="J20" s="1">
         <v>28</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K20" s="1">
+        <v>190</v>
+      </c>
+      <c r="L20" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -3000,8 +3127,14 @@
       <c r="J21" s="1">
         <v>29</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K21" s="1">
+        <v>200</v>
+      </c>
+      <c r="L21" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -3023,8 +3156,14 @@
       <c r="J22" s="1">
         <v>30</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K22" s="1">
+        <v>210</v>
+      </c>
+      <c r="L22" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -3046,8 +3185,14 @@
       <c r="J23" s="1">
         <v>31</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K23" s="1">
+        <v>220</v>
+      </c>
+      <c r="L23" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -3069,8 +3214,14 @@
       <c r="J24" s="1">
         <v>32</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K24" s="1">
+        <v>230</v>
+      </c>
+      <c r="L24" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -3092,8 +3243,14 @@
       <c r="J25" s="1">
         <v>33</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K25" s="1">
+        <v>240</v>
+      </c>
+      <c r="L25" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -3115,8 +3272,14 @@
       <c r="J26" s="1">
         <v>34</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K26" s="1">
+        <v>250</v>
+      </c>
+      <c r="L26" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -3138,8 +3301,14 @@
       <c r="J27" s="1">
         <v>35</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K27" s="1">
+        <v>260</v>
+      </c>
+      <c r="L27" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -3161,8 +3330,14 @@
       <c r="J28" s="1">
         <v>36</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K28" s="1">
+        <v>270</v>
+      </c>
+      <c r="L28" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -3184,8 +3359,14 @@
       <c r="J29" s="1">
         <v>37</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K29" s="1">
+        <v>280</v>
+      </c>
+      <c r="L29" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -3207,8 +3388,14 @@
       <c r="J30" s="1">
         <v>38</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K30" s="1">
+        <v>290</v>
+      </c>
+      <c r="L30" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -3230,8 +3417,14 @@
       <c r="J31" s="1">
         <v>39</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K31" s="1">
+        <v>300</v>
+      </c>
+      <c r="L31" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -3253,8 +3446,14 @@
       <c r="J32" s="1">
         <v>40</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K32" s="1">
+        <v>310</v>
+      </c>
+      <c r="L32" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -3276,8 +3475,14 @@
       <c r="J33" s="1">
         <v>41</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K33" s="1">
+        <v>320</v>
+      </c>
+      <c r="L33" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -3299,8 +3504,14 @@
       <c r="J34" s="1">
         <v>42</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K34" s="1">
+        <v>330</v>
+      </c>
+      <c r="L34" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -3322,8 +3533,14 @@
       <c r="J35" s="1">
         <v>43</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K35" s="1">
+        <v>340</v>
+      </c>
+      <c r="L35" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -3345,8 +3562,14 @@
       <c r="J36" s="1">
         <v>44</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K36" s="1">
+        <v>350</v>
+      </c>
+      <c r="L36" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -3368,8 +3591,14 @@
       <c r="J37" s="1">
         <v>45</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K37" s="1">
+        <v>360</v>
+      </c>
+      <c r="L37" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -3391,8 +3620,14 @@
       <c r="J38" s="1">
         <v>46</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K38" s="1">
+        <v>370</v>
+      </c>
+      <c r="L38" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -3414,8 +3649,14 @@
       <c r="J39" s="1">
         <v>47</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K39" s="1">
+        <v>380</v>
+      </c>
+      <c r="L39" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -3437,15 +3678,21 @@
       <c r="J40" s="1">
         <v>48</v>
       </c>
+      <c r="K40" s="1">
+        <v>390</v>
+      </c>
+      <c r="L40" s="1">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="M2:M14"/>
+    <mergeCell ref="N2:N14"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
-      <formula1>$N$2:$N$962</formula1>
+      <formula1>$O$2:$O$962</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.69999998807907104" right="0.69999998807907104" top="0.75" bottom="0.75" header="0.30000001192092896" footer="0.30000001192092896"/>
@@ -3459,10 +3706,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{538B65EF-D419-4214-A215-575E19AD76B9}">
-  <dimension ref="A1:L57"/>
+  <dimension ref="A1:O57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3477,12 +3724,13 @@
     <col min="8" max="8" width="17.375" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.5" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="21.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="32.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9" style="1"/>
+    <col min="11" max="13" width="21.75" style="1" customWidth="1"/>
+    <col min="14" max="14" width="9.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="32.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -3513,14 +3761,21 @@
       <c r="J1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="M1" s="5"/>
+      <c r="N1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <f>MonsterBaseData!A2</f>
         <v>1</v>
@@ -3553,9 +3808,17 @@
         <f>MonsterBaseData!J2*1.5</f>
         <v>15</v>
       </c>
-      <c r="K2" s="7"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K2" s="1">
+        <f>MonsterBaseData!K2</f>
+        <v>10</v>
+      </c>
+      <c r="L2" s="1">
+        <f>MonsterBaseData!L2</f>
+        <v>1</v>
+      </c>
+      <c r="N2" s="7"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <f>MonsterBaseData!A3</f>
         <v>2</v>
@@ -3588,9 +3851,17 @@
         <f>MonsterBaseData!J3*1.5</f>
         <v>16.5</v>
       </c>
-      <c r="K3" s="7"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K3" s="1">
+        <f>MonsterBaseData!K3</f>
+        <v>20</v>
+      </c>
+      <c r="L3" s="1">
+        <f>MonsterBaseData!L3</f>
+        <v>1</v>
+      </c>
+      <c r="N3" s="7"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <f>MonsterBaseData!A4</f>
         <v>3</v>
@@ -3623,9 +3894,17 @@
         <f>MonsterBaseData!J4*1.5</f>
         <v>18</v>
       </c>
-      <c r="K4" s="7"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K4" s="1">
+        <f>MonsterBaseData!K4</f>
+        <v>30</v>
+      </c>
+      <c r="L4" s="1">
+        <f>MonsterBaseData!L4</f>
+        <v>1</v>
+      </c>
+      <c r="N4" s="7"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <f>MonsterBaseData!A5</f>
         <v>4</v>
@@ -3658,9 +3937,17 @@
         <f>MonsterBaseData!J5*1.5</f>
         <v>19.5</v>
       </c>
-      <c r="K5" s="7"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K5" s="1">
+        <f>MonsterBaseData!K5</f>
+        <v>40</v>
+      </c>
+      <c r="L5" s="1">
+        <f>MonsterBaseData!L5</f>
+        <v>1</v>
+      </c>
+      <c r="N5" s="7"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <f>MonsterBaseData!A6</f>
         <v>5</v>
@@ -3693,9 +3980,17 @@
         <f>MonsterBaseData!J6*1.5</f>
         <v>21</v>
       </c>
-      <c r="K6" s="7"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K6" s="1">
+        <f>MonsterBaseData!K6</f>
+        <v>50</v>
+      </c>
+      <c r="L6" s="1">
+        <f>MonsterBaseData!L6</f>
+        <v>1</v>
+      </c>
+      <c r="N6" s="7"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <f>MonsterBaseData!A7</f>
         <v>6</v>
@@ -3728,9 +4023,17 @@
         <f>MonsterBaseData!J7*1.5</f>
         <v>22.5</v>
       </c>
-      <c r="K7" s="7"/>
-    </row>
-    <row r="8" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K7" s="1">
+        <f>MonsterBaseData!K7</f>
+        <v>60</v>
+      </c>
+      <c r="L7" s="1">
+        <f>MonsterBaseData!L7</f>
+        <v>1</v>
+      </c>
+      <c r="N7" s="7"/>
+    </row>
+    <row r="8" spans="1:15" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <f>MonsterBaseData!A8</f>
         <v>7</v>
@@ -3763,9 +4066,17 @@
         <f>MonsterBaseData!J8*1.5</f>
         <v>24</v>
       </c>
-      <c r="K8" s="7"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K8" s="1">
+        <f>MonsterBaseData!K8</f>
+        <v>70</v>
+      </c>
+      <c r="L8" s="1">
+        <f>MonsterBaseData!L8</f>
+        <v>1</v>
+      </c>
+      <c r="N8" s="7"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <f>MonsterBaseData!A9</f>
         <v>8</v>
@@ -3798,9 +4109,17 @@
         <f>MonsterBaseData!J9*1.5</f>
         <v>25.5</v>
       </c>
-      <c r="K9" s="8"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K9" s="1">
+        <f>MonsterBaseData!K9</f>
+        <v>80</v>
+      </c>
+      <c r="L9" s="1">
+        <f>MonsterBaseData!L9</f>
+        <v>1</v>
+      </c>
+      <c r="N9" s="8"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <f>MonsterBaseData!A10</f>
         <v>9</v>
@@ -3833,9 +4152,17 @@
         <f>MonsterBaseData!J10*1.5</f>
         <v>27</v>
       </c>
-      <c r="K10" s="8"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K10" s="1">
+        <f>MonsterBaseData!K10</f>
+        <v>90</v>
+      </c>
+      <c r="L10" s="1">
+        <f>MonsterBaseData!L10</f>
+        <v>1</v>
+      </c>
+      <c r="N10" s="8"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <f>MonsterBaseData!A11</f>
         <v>10</v>
@@ -3868,9 +4195,17 @@
         <f>MonsterBaseData!J11*1.5</f>
         <v>28.5</v>
       </c>
-      <c r="K11" s="8"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K11" s="1">
+        <f>MonsterBaseData!K11</f>
+        <v>100</v>
+      </c>
+      <c r="L11" s="1">
+        <f>MonsterBaseData!L11</f>
+        <v>1</v>
+      </c>
+      <c r="N11" s="8"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <f>MonsterBaseData!A12</f>
         <v>11</v>
@@ -3903,9 +4238,17 @@
         <f>MonsterBaseData!J12*1.5</f>
         <v>30</v>
       </c>
-      <c r="K12" s="8"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K12" s="1">
+        <f>MonsterBaseData!K12</f>
+        <v>110</v>
+      </c>
+      <c r="L12" s="1">
+        <f>MonsterBaseData!L12</f>
+        <v>1</v>
+      </c>
+      <c r="N12" s="8"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <f>MonsterBaseData!A13</f>
         <v>12</v>
@@ -3938,9 +4281,17 @@
         <f>MonsterBaseData!J13*1.5</f>
         <v>31.5</v>
       </c>
-      <c r="K13" s="8"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K13" s="1">
+        <f>MonsterBaseData!K13</f>
+        <v>120</v>
+      </c>
+      <c r="L13" s="1">
+        <f>MonsterBaseData!L13</f>
+        <v>1</v>
+      </c>
+      <c r="N13" s="8"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <f>MonsterBaseData!A14</f>
         <v>13</v>
@@ -3973,9 +4324,17 @@
         <f>MonsterBaseData!J14*1.5</f>
         <v>33</v>
       </c>
-      <c r="K14" s="8"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K14" s="1">
+        <f>MonsterBaseData!K14</f>
+        <v>130</v>
+      </c>
+      <c r="L14" s="1">
+        <f>MonsterBaseData!L14</f>
+        <v>1</v>
+      </c>
+      <c r="N14" s="8"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <f>MonsterBaseData!A15</f>
         <v>14</v>
@@ -4008,8 +4367,16 @@
         <f>MonsterBaseData!J15*1.5</f>
         <v>34.5</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K15" s="1">
+        <f>MonsterBaseData!K15</f>
+        <v>140</v>
+      </c>
+      <c r="L15" s="1">
+        <f>MonsterBaseData!L15</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <f>MonsterBaseData!A16</f>
         <v>15</v>
@@ -4042,8 +4409,16 @@
         <f>MonsterBaseData!J16*1.5</f>
         <v>36</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K16" s="1">
+        <f>MonsterBaseData!K16</f>
+        <v>150</v>
+      </c>
+      <c r="L16" s="1">
+        <f>MonsterBaseData!L16</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <f>MonsterBaseData!A17</f>
         <v>16</v>
@@ -4076,8 +4451,16 @@
         <f>MonsterBaseData!J17*1.5</f>
         <v>37.5</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K17" s="1">
+        <f>MonsterBaseData!K17</f>
+        <v>160</v>
+      </c>
+      <c r="L17" s="1">
+        <f>MonsterBaseData!L17</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <f>MonsterBaseData!A18</f>
         <v>17</v>
@@ -4110,8 +4493,16 @@
         <f>MonsterBaseData!J18*1.5</f>
         <v>39</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K18" s="1">
+        <f>MonsterBaseData!K18</f>
+        <v>170</v>
+      </c>
+      <c r="L18" s="1">
+        <f>MonsterBaseData!L18</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <f>MonsterBaseData!A19</f>
         <v>18</v>
@@ -4144,8 +4535,16 @@
         <f>MonsterBaseData!J19*1.5</f>
         <v>40.5</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K19" s="1">
+        <f>MonsterBaseData!K19</f>
+        <v>180</v>
+      </c>
+      <c r="L19" s="1">
+        <f>MonsterBaseData!L19</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <f>MonsterBaseData!A20</f>
         <v>19</v>
@@ -4178,8 +4577,16 @@
         <f>MonsterBaseData!J20*1.5</f>
         <v>42</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K20" s="1">
+        <f>MonsterBaseData!K20</f>
+        <v>190</v>
+      </c>
+      <c r="L20" s="1">
+        <f>MonsterBaseData!L20</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <f>MonsterBaseData!A21</f>
         <v>20</v>
@@ -4212,8 +4619,16 @@
         <f>MonsterBaseData!J21*1.5</f>
         <v>43.5</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K21" s="1">
+        <f>MonsterBaseData!K21</f>
+        <v>200</v>
+      </c>
+      <c r="L21" s="1">
+        <f>MonsterBaseData!L21</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <f>MonsterBaseData!A22</f>
         <v>21</v>
@@ -4246,8 +4661,16 @@
         <f>MonsterBaseData!J22*1.5</f>
         <v>45</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K22" s="1">
+        <f>MonsterBaseData!K22</f>
+        <v>210</v>
+      </c>
+      <c r="L22" s="1">
+        <f>MonsterBaseData!L22</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <f>MonsterBaseData!A23</f>
         <v>22</v>
@@ -4280,8 +4703,16 @@
         <f>MonsterBaseData!J23*1.5</f>
         <v>46.5</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K23" s="1">
+        <f>MonsterBaseData!K23</f>
+        <v>220</v>
+      </c>
+      <c r="L23" s="1">
+        <f>MonsterBaseData!L23</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <f>MonsterBaseData!A24</f>
         <v>23</v>
@@ -4314,8 +4745,16 @@
         <f>MonsterBaseData!J24*1.5</f>
         <v>48</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K24" s="1">
+        <f>MonsterBaseData!K24</f>
+        <v>230</v>
+      </c>
+      <c r="L24" s="1">
+        <f>MonsterBaseData!L24</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <f>MonsterBaseData!A25</f>
         <v>24</v>
@@ -4348,8 +4787,16 @@
         <f>MonsterBaseData!J25*1.5</f>
         <v>49.5</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K25" s="1">
+        <f>MonsterBaseData!K25</f>
+        <v>240</v>
+      </c>
+      <c r="L25" s="1">
+        <f>MonsterBaseData!L25</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <f>MonsterBaseData!A26</f>
         <v>25</v>
@@ -4382,8 +4829,16 @@
         <f>MonsterBaseData!J26*1.5</f>
         <v>51</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K26" s="1">
+        <f>MonsterBaseData!K26</f>
+        <v>250</v>
+      </c>
+      <c r="L26" s="1">
+        <f>MonsterBaseData!L26</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <f>MonsterBaseData!A27</f>
         <v>26</v>
@@ -4416,8 +4871,16 @@
         <f>MonsterBaseData!J27*1.5</f>
         <v>52.5</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K27" s="1">
+        <f>MonsterBaseData!K27</f>
+        <v>260</v>
+      </c>
+      <c r="L27" s="1">
+        <f>MonsterBaseData!L27</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <f>MonsterBaseData!A28</f>
         <v>27</v>
@@ -4450,8 +4913,16 @@
         <f>MonsterBaseData!J28*1.5</f>
         <v>54</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K28" s="1">
+        <f>MonsterBaseData!K28</f>
+        <v>270</v>
+      </c>
+      <c r="L28" s="1">
+        <f>MonsterBaseData!L28</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <f>MonsterBaseData!A29</f>
         <v>28</v>
@@ -4484,8 +4955,16 @@
         <f>MonsterBaseData!J29*1.5</f>
         <v>55.5</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K29" s="1">
+        <f>MonsterBaseData!K29</f>
+        <v>280</v>
+      </c>
+      <c r="L29" s="1">
+        <f>MonsterBaseData!L29</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <f>MonsterBaseData!A30</f>
         <v>29</v>
@@ -4518,8 +4997,16 @@
         <f>MonsterBaseData!J30*1.5</f>
         <v>57</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K30" s="1">
+        <f>MonsterBaseData!K30</f>
+        <v>290</v>
+      </c>
+      <c r="L30" s="1">
+        <f>MonsterBaseData!L30</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <f>MonsterBaseData!A31</f>
         <v>30</v>
@@ -4552,8 +5039,16 @@
         <f>MonsterBaseData!J31*1.5</f>
         <v>58.5</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K31" s="1">
+        <f>MonsterBaseData!K31</f>
+        <v>300</v>
+      </c>
+      <c r="L31" s="1">
+        <f>MonsterBaseData!L31</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <f>MonsterBaseData!A32</f>
         <v>31</v>
@@ -4586,8 +5081,16 @@
         <f>MonsterBaseData!J32*1.5</f>
         <v>60</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K32" s="1">
+        <f>MonsterBaseData!K32</f>
+        <v>310</v>
+      </c>
+      <c r="L32" s="1">
+        <f>MonsterBaseData!L32</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <f>MonsterBaseData!A33</f>
         <v>32</v>
@@ -4620,8 +5123,16 @@
         <f>MonsterBaseData!J33*1.5</f>
         <v>61.5</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K33" s="1">
+        <f>MonsterBaseData!K33</f>
+        <v>320</v>
+      </c>
+      <c r="L33" s="1">
+        <f>MonsterBaseData!L33</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <f>MonsterBaseData!A34</f>
         <v>33</v>
@@ -4654,8 +5165,16 @@
         <f>MonsterBaseData!J34*1.5</f>
         <v>63</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K34" s="1">
+        <f>MonsterBaseData!K34</f>
+        <v>330</v>
+      </c>
+      <c r="L34" s="1">
+        <f>MonsterBaseData!L34</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <f>MonsterBaseData!A35</f>
         <v>34</v>
@@ -4688,8 +5207,16 @@
         <f>MonsterBaseData!J35*1.5</f>
         <v>64.5</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K35" s="1">
+        <f>MonsterBaseData!K35</f>
+        <v>340</v>
+      </c>
+      <c r="L35" s="1">
+        <f>MonsterBaseData!L35</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <f>MonsterBaseData!A36</f>
         <v>35</v>
@@ -4722,8 +5249,16 @@
         <f>MonsterBaseData!J36*1.5</f>
         <v>66</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K36" s="1">
+        <f>MonsterBaseData!K36</f>
+        <v>350</v>
+      </c>
+      <c r="L36" s="1">
+        <f>MonsterBaseData!L36</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <f>MonsterBaseData!A37</f>
         <v>36</v>
@@ -4756,8 +5291,16 @@
         <f>MonsterBaseData!J37*1.5</f>
         <v>67.5</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K37" s="1">
+        <f>MonsterBaseData!K37</f>
+        <v>360</v>
+      </c>
+      <c r="L37" s="1">
+        <f>MonsterBaseData!L37</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <f>MonsterBaseData!A38</f>
         <v>37</v>
@@ -4790,8 +5333,16 @@
         <f>MonsterBaseData!J38*1.5</f>
         <v>69</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K38" s="1">
+        <f>MonsterBaseData!K38</f>
+        <v>370</v>
+      </c>
+      <c r="L38" s="1">
+        <f>MonsterBaseData!L38</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <f>MonsterBaseData!A39</f>
         <v>38</v>
@@ -4824,8 +5375,16 @@
         <f>MonsterBaseData!J39*1.5</f>
         <v>70.5</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K39" s="1">
+        <f>MonsterBaseData!K39</f>
+        <v>380</v>
+      </c>
+      <c r="L39" s="1">
+        <f>MonsterBaseData!L39</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <f>MonsterBaseData!A40</f>
         <v>39</v>
@@ -4858,29 +5417,37 @@
         <f>MonsterBaseData!J40*1.5</f>
         <v>72</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K40" s="1">
+        <f>MonsterBaseData!K40</f>
+        <v>390</v>
+      </c>
+      <c r="L40" s="1">
+        <f>MonsterBaseData!L40</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C41" s="1"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C42" s="1"/>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C43" s="1"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C44" s="1"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C45" s="1"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C46" s="1"/>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C47" s="1"/>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C48" s="1"/>
     </row>
     <row r="49" spans="3:3" x14ac:dyDescent="0.3">
@@ -4912,12 +5479,12 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="K2:K14"/>
+    <mergeCell ref="N2:N14"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B58:B1048576" xr:uid="{3F7F906E-6C9A-4B61-8B66-8773D370EC07}">
-      <formula1>$L$2:$L$962</formula1>
+      <formula1>$O$2:$O$962</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4930,10 +5497,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F360BF2-F57C-43E4-A45B-98C9530388AF}">
-  <dimension ref="A1:K40"/>
+  <dimension ref="A1:N40"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4948,11 +5515,12 @@
     <col min="8" max="8" width="20.125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17.5" style="1" customWidth="1"/>
     <col min="10" max="10" width="21.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="32.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9" style="1"/>
+    <col min="11" max="13" width="21.75" style="1" customWidth="1"/>
+    <col min="14" max="14" width="32.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -4983,11 +5551,18 @@
       <c r="J1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="M1" s="5"/>
+      <c r="N1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <f>MonsterBaseData!A2</f>
         <v>1</v>
@@ -5020,8 +5595,16 @@
         <f>MonsterBaseData!J2</f>
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K2" s="1">
+        <f>MonsterBaseData!K2</f>
+        <v>10</v>
+      </c>
+      <c r="L2" s="1">
+        <f>MonsterBaseData!L2*10</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <f>MonsterBaseData!A3</f>
         <v>2</v>
@@ -5054,8 +5637,16 @@
         <f>MonsterBaseData!J3</f>
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K3" s="1">
+        <f>MonsterBaseData!K3</f>
+        <v>20</v>
+      </c>
+      <c r="L3" s="1">
+        <f>MonsterBaseData!L3*10</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <f>MonsterBaseData!A4</f>
         <v>3</v>
@@ -5088,8 +5679,16 @@
         <f>MonsterBaseData!J4</f>
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K4" s="1">
+        <f>MonsterBaseData!K4</f>
+        <v>30</v>
+      </c>
+      <c r="L4" s="1">
+        <f>MonsterBaseData!L4*10</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <f>MonsterBaseData!A5</f>
         <v>4</v>
@@ -5122,8 +5721,16 @@
         <f>MonsterBaseData!J5</f>
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K5" s="1">
+        <f>MonsterBaseData!K5</f>
+        <v>40</v>
+      </c>
+      <c r="L5" s="1">
+        <f>MonsterBaseData!L5*10</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <f>MonsterBaseData!A6</f>
         <v>5</v>
@@ -5156,8 +5763,16 @@
         <f>MonsterBaseData!J6</f>
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K6" s="1">
+        <f>MonsterBaseData!K6</f>
+        <v>50</v>
+      </c>
+      <c r="L6" s="1">
+        <f>MonsterBaseData!L6*10</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <f>MonsterBaseData!A7</f>
         <v>6</v>
@@ -5190,8 +5805,16 @@
         <f>MonsterBaseData!J7</f>
         <v>15</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K7" s="1">
+        <f>MonsterBaseData!K7</f>
+        <v>60</v>
+      </c>
+      <c r="L7" s="1">
+        <f>MonsterBaseData!L7*10</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <f>MonsterBaseData!A8</f>
         <v>7</v>
@@ -5224,8 +5847,16 @@
         <f>MonsterBaseData!J8</f>
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K8" s="1">
+        <f>MonsterBaseData!K8</f>
+        <v>70</v>
+      </c>
+      <c r="L8" s="1">
+        <f>MonsterBaseData!L8*10</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <f>MonsterBaseData!A9</f>
         <v>8</v>
@@ -5258,8 +5889,16 @@
         <f>MonsterBaseData!J9</f>
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K9" s="1">
+        <f>MonsterBaseData!K9</f>
+        <v>80</v>
+      </c>
+      <c r="L9" s="1">
+        <f>MonsterBaseData!L9*10</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <f>MonsterBaseData!A10</f>
         <v>9</v>
@@ -5292,8 +5931,16 @@
         <f>MonsterBaseData!J10</f>
         <v>18</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K10" s="1">
+        <f>MonsterBaseData!K10</f>
+        <v>90</v>
+      </c>
+      <c r="L10" s="1">
+        <f>MonsterBaseData!L10*10</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <f>MonsterBaseData!A11</f>
         <v>10</v>
@@ -5326,8 +5973,16 @@
         <f>MonsterBaseData!J11</f>
         <v>19</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K11" s="1">
+        <f>MonsterBaseData!K11</f>
+        <v>100</v>
+      </c>
+      <c r="L11" s="1">
+        <f>MonsterBaseData!L11*10</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <f>MonsterBaseData!A12</f>
         <v>11</v>
@@ -5360,8 +6015,16 @@
         <f>MonsterBaseData!J12</f>
         <v>20</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K12" s="1">
+        <f>MonsterBaseData!K12</f>
+        <v>110</v>
+      </c>
+      <c r="L12" s="1">
+        <f>MonsterBaseData!L12*10</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <f>MonsterBaseData!A13</f>
         <v>12</v>
@@ -5394,8 +6057,16 @@
         <f>MonsterBaseData!J13</f>
         <v>21</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K13" s="1">
+        <f>MonsterBaseData!K13</f>
+        <v>120</v>
+      </c>
+      <c r="L13" s="1">
+        <f>MonsterBaseData!L13*10</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <f>MonsterBaseData!A14</f>
         <v>13</v>
@@ -5428,8 +6099,16 @@
         <f>MonsterBaseData!J14</f>
         <v>22</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K14" s="1">
+        <f>MonsterBaseData!K14</f>
+        <v>130</v>
+      </c>
+      <c r="L14" s="1">
+        <f>MonsterBaseData!L14*10</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <f>MonsterBaseData!A15</f>
         <v>14</v>
@@ -5462,8 +6141,16 @@
         <f>MonsterBaseData!J15</f>
         <v>23</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K15" s="1">
+        <f>MonsterBaseData!K15</f>
+        <v>140</v>
+      </c>
+      <c r="L15" s="1">
+        <f>MonsterBaseData!L15*10</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <f>MonsterBaseData!A16</f>
         <v>15</v>
@@ -5496,8 +6183,16 @@
         <f>MonsterBaseData!J16</f>
         <v>24</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K16" s="1">
+        <f>MonsterBaseData!K16</f>
+        <v>150</v>
+      </c>
+      <c r="L16" s="1">
+        <f>MonsterBaseData!L16*10</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <f>MonsterBaseData!A17</f>
         <v>16</v>
@@ -5530,8 +6225,16 @@
         <f>MonsterBaseData!J17</f>
         <v>25</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K17" s="1">
+        <f>MonsterBaseData!K17</f>
+        <v>160</v>
+      </c>
+      <c r="L17" s="1">
+        <f>MonsterBaseData!L17*10</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <f>MonsterBaseData!A18</f>
         <v>17</v>
@@ -5564,8 +6267,16 @@
         <f>MonsterBaseData!J18</f>
         <v>26</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K18" s="1">
+        <f>MonsterBaseData!K18</f>
+        <v>170</v>
+      </c>
+      <c r="L18" s="1">
+        <f>MonsterBaseData!L18*10</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <f>MonsterBaseData!A19</f>
         <v>18</v>
@@ -5598,8 +6309,16 @@
         <f>MonsterBaseData!J19</f>
         <v>27</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K19" s="1">
+        <f>MonsterBaseData!K19</f>
+        <v>180</v>
+      </c>
+      <c r="L19" s="1">
+        <f>MonsterBaseData!L19*10</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <f>MonsterBaseData!A20</f>
         <v>19</v>
@@ -5632,8 +6351,16 @@
         <f>MonsterBaseData!J20</f>
         <v>28</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K20" s="1">
+        <f>MonsterBaseData!K20</f>
+        <v>190</v>
+      </c>
+      <c r="L20" s="1">
+        <f>MonsterBaseData!L20*10</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <f>MonsterBaseData!A21</f>
         <v>20</v>
@@ -5666,8 +6393,16 @@
         <f>MonsterBaseData!J21</f>
         <v>29</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K21" s="1">
+        <f>MonsterBaseData!K21</f>
+        <v>200</v>
+      </c>
+      <c r="L21" s="1">
+        <f>MonsterBaseData!L21*10</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <f>MonsterBaseData!A22</f>
         <v>21</v>
@@ -5700,8 +6435,16 @@
         <f>MonsterBaseData!J22</f>
         <v>30</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K22" s="1">
+        <f>MonsterBaseData!K22</f>
+        <v>210</v>
+      </c>
+      <c r="L22" s="1">
+        <f>MonsterBaseData!L22*10</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <f>MonsterBaseData!A23</f>
         <v>22</v>
@@ -5734,8 +6477,16 @@
         <f>MonsterBaseData!J23</f>
         <v>31</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K23" s="1">
+        <f>MonsterBaseData!K23</f>
+        <v>220</v>
+      </c>
+      <c r="L23" s="1">
+        <f>MonsterBaseData!L23*10</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <f>MonsterBaseData!A24</f>
         <v>23</v>
@@ -5768,8 +6519,16 @@
         <f>MonsterBaseData!J24</f>
         <v>32</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K24" s="1">
+        <f>MonsterBaseData!K24</f>
+        <v>230</v>
+      </c>
+      <c r="L24" s="1">
+        <f>MonsterBaseData!L24*10</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <f>MonsterBaseData!A25</f>
         <v>24</v>
@@ -5802,8 +6561,16 @@
         <f>MonsterBaseData!J25</f>
         <v>33</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K25" s="1">
+        <f>MonsterBaseData!K25</f>
+        <v>240</v>
+      </c>
+      <c r="L25" s="1">
+        <f>MonsterBaseData!L25*10</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <f>MonsterBaseData!A26</f>
         <v>25</v>
@@ -5836,8 +6603,16 @@
         <f>MonsterBaseData!J26</f>
         <v>34</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K26" s="1">
+        <f>MonsterBaseData!K26</f>
+        <v>250</v>
+      </c>
+      <c r="L26" s="1">
+        <f>MonsterBaseData!L26*10</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <f>MonsterBaseData!A27</f>
         <v>26</v>
@@ -5870,8 +6645,16 @@
         <f>MonsterBaseData!J27</f>
         <v>35</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K27" s="1">
+        <f>MonsterBaseData!K27</f>
+        <v>260</v>
+      </c>
+      <c r="L27" s="1">
+        <f>MonsterBaseData!L27*10</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <f>MonsterBaseData!A28</f>
         <v>27</v>
@@ -5904,8 +6687,16 @@
         <f>MonsterBaseData!J28</f>
         <v>36</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K28" s="1">
+        <f>MonsterBaseData!K28</f>
+        <v>270</v>
+      </c>
+      <c r="L28" s="1">
+        <f>MonsterBaseData!L28*10</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <f>MonsterBaseData!A29</f>
         <v>28</v>
@@ -5938,8 +6729,16 @@
         <f>MonsterBaseData!J29</f>
         <v>37</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K29" s="1">
+        <f>MonsterBaseData!K29</f>
+        <v>280</v>
+      </c>
+      <c r="L29" s="1">
+        <f>MonsterBaseData!L29*10</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <f>MonsterBaseData!A30</f>
         <v>29</v>
@@ -5972,8 +6771,16 @@
         <f>MonsterBaseData!J30</f>
         <v>38</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K30" s="1">
+        <f>MonsterBaseData!K30</f>
+        <v>290</v>
+      </c>
+      <c r="L30" s="1">
+        <f>MonsterBaseData!L30*10</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <f>MonsterBaseData!A31</f>
         <v>30</v>
@@ -6006,8 +6813,16 @@
         <f>MonsterBaseData!J31</f>
         <v>39</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K31" s="1">
+        <f>MonsterBaseData!K31</f>
+        <v>300</v>
+      </c>
+      <c r="L31" s="1">
+        <f>MonsterBaseData!L31*10</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <f>MonsterBaseData!A32</f>
         <v>31</v>
@@ -6040,8 +6855,16 @@
         <f>MonsterBaseData!J32</f>
         <v>40</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K32" s="1">
+        <f>MonsterBaseData!K32</f>
+        <v>310</v>
+      </c>
+      <c r="L32" s="1">
+        <f>MonsterBaseData!L32*10</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <f>MonsterBaseData!A33</f>
         <v>32</v>
@@ -6074,8 +6897,16 @@
         <f>MonsterBaseData!J33</f>
         <v>41</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K33" s="1">
+        <f>MonsterBaseData!K33</f>
+        <v>320</v>
+      </c>
+      <c r="L33" s="1">
+        <f>MonsterBaseData!L33*10</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <f>MonsterBaseData!A34</f>
         <v>33</v>
@@ -6108,8 +6939,16 @@
         <f>MonsterBaseData!J34</f>
         <v>42</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K34" s="1">
+        <f>MonsterBaseData!K34</f>
+        <v>330</v>
+      </c>
+      <c r="L34" s="1">
+        <f>MonsterBaseData!L34*10</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <f>MonsterBaseData!A35</f>
         <v>34</v>
@@ -6142,8 +6981,16 @@
         <f>MonsterBaseData!J35</f>
         <v>43</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K35" s="1">
+        <f>MonsterBaseData!K35</f>
+        <v>340</v>
+      </c>
+      <c r="L35" s="1">
+        <f>MonsterBaseData!L35*10</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <f>MonsterBaseData!A36</f>
         <v>35</v>
@@ -6176,8 +7023,16 @@
         <f>MonsterBaseData!J36</f>
         <v>44</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K36" s="1">
+        <f>MonsterBaseData!K36</f>
+        <v>350</v>
+      </c>
+      <c r="L36" s="1">
+        <f>MonsterBaseData!L36*10</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <f>MonsterBaseData!A37</f>
         <v>36</v>
@@ -6210,8 +7065,16 @@
         <f>MonsterBaseData!J37</f>
         <v>45</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K37" s="1">
+        <f>MonsterBaseData!K37</f>
+        <v>360</v>
+      </c>
+      <c r="L37" s="1">
+        <f>MonsterBaseData!L37*10</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <f>MonsterBaseData!A38</f>
         <v>37</v>
@@ -6244,8 +7107,16 @@
         <f>MonsterBaseData!J38</f>
         <v>46</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K38" s="1">
+        <f>MonsterBaseData!K38</f>
+        <v>370</v>
+      </c>
+      <c r="L38" s="1">
+        <f>MonsterBaseData!L38*10</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <f>MonsterBaseData!A39</f>
         <v>38</v>
@@ -6278,8 +7149,16 @@
         <f>MonsterBaseData!J39</f>
         <v>47</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K39" s="1">
+        <f>MonsterBaseData!K39</f>
+        <v>380</v>
+      </c>
+      <c r="L39" s="1">
+        <f>MonsterBaseData!L39*10</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <f>MonsterBaseData!A40</f>
         <v>39</v>
@@ -6311,13 +7190,21 @@
       <c r="J40" s="1">
         <f>MonsterBaseData!J40</f>
         <v>48</v>
+      </c>
+      <c r="K40" s="1">
+        <f>MonsterBaseData!K40</f>
+        <v>390</v>
+      </c>
+      <c r="L40" s="1">
+        <f>MonsterBaseData!L40*10</f>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B41:B1048576" xr:uid="{00A1E1D4-7382-459B-BF8F-8C45AF75A2DE}">
-      <formula1>$K$2:$K$962</formula1>
+      <formula1>$N$2:$N$962</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>